<commit_message>
actualizacion de requisitos e historias
</commit_message>
<xml_diff>
--- a/documentacion/scrum/Product backlog.xlsx
+++ b/documentacion/scrum/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyecto\documentacion\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3663B5C5-29AA-43D6-AB43-902001666C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FCB278-DA70-41AD-8576-7ACC547B1480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{62494E98-7055-48D3-B966-884A22B78DF5}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="107">
   <si>
     <t>Product backlog</t>
   </si>
@@ -159,12 +159,6 @@
     <t>HU13</t>
   </si>
   <si>
-    <t>Registrar cliente</t>
-  </si>
-  <si>
-    <t>Autenticar usuario</t>
-  </si>
-  <si>
     <t>Visualizar y modificar datos del usuario</t>
   </si>
   <si>
@@ -358,6 +352,15 @@
   </si>
   <si>
     <t>Despliegue y puesta a punto</t>
+  </si>
+  <si>
+    <t>Añadir historias de usuario faltantes</t>
+  </si>
+  <si>
+    <t>Gestionar registro y autenticacion de usuarios</t>
+  </si>
+  <si>
+    <t>Visualizar panel de inicio</t>
   </si>
 </sst>
 </file>
@@ -387,7 +390,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,6 +418,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -543,6 +552,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -552,6 +565,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -567,6 +583,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -579,6 +601,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -594,10 +622,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,7 +977,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -950,12 +992,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -968,16 +1010,16 @@
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="F2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -992,19 +1034,19 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="I3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="I3" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1022,19 +1064,19 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G4" s="2">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1051,19 +1093,19 @@
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G5" s="2">
         <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1079,6 +1121,21 @@
       <c r="D6" s="2">
         <v>2</v>
       </c>
+      <c r="F6" s="34">
+        <v>45394</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="35" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
@@ -1127,7 +1184,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>14</v>
@@ -1155,7 +1212,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>14</v>
@@ -1169,13 +1226,13 @@
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1183,13 +1240,13 @@
         <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -1197,7 +1254,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>14</v>
@@ -1211,7 +1268,7 @@
         <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>14</v>
@@ -1222,10 +1279,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>14</v>
@@ -1236,10 +1293,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>14</v>
@@ -1253,7 +1310,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>14</v>
@@ -1267,7 +1324,7 @@
         <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>14</v>
@@ -1281,7 +1338,7 @@
         <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>14</v>
@@ -1295,7 +1352,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>14</v>
@@ -1306,10 +1363,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>14</v>
@@ -1320,13 +1377,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D24" s="2">
         <v>2</v>
@@ -1348,13 +1405,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D26" s="2">
         <v>6</v>
@@ -1365,10 +1422,10 @@
         <v>38</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
@@ -1379,10 +1436,10 @@
         <v>33</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D28" s="2">
         <v>2</v>
@@ -1393,7 +1450,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>24</v>
@@ -1404,13 +1461,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30" s="2">
         <v>2</v>
@@ -1418,13 +1475,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D31" s="2">
         <v>2</v>
@@ -1432,10 +1489,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>24</v>
@@ -1449,7 +1506,7 @@
         <v>23</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>24</v>
@@ -1460,10 +1517,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>24</v>
@@ -1487,8 +1544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49D8E50-E16B-43C7-A737-D72E991DFD2E}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1505,57 +1562,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="21">
+      <c r="A4" s="26">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="str">
@@ -1566,25 +1623,25 @@
         <f>'Product backlog'!B3</f>
         <v>Instalar las herramientas de desarrollo</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="21">
+      <c r="D4" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="26">
         <v>6</v>
       </c>
       <c r="G4" s="2">
         <f>'Product backlog'!D3</f>
         <v>1</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="26">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="21"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="2" t="str">
         <f>'Product backlog'!A4</f>
         <v>HT2</v>
@@ -1593,17 +1650,17 @@
         <f>'Product backlog'!B4</f>
         <v>Establecer el estándar de codificación</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="2">
         <f>'Product backlog'!D4</f>
         <v>1</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="2" t="str">
         <f>'Product backlog'!A5</f>
         <v>HT3</v>
@@ -1612,24 +1669,24 @@
         <f>'Product backlog'!B5</f>
         <v>Establecer el diseño de base de datos</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="2">
         <f>'Product backlog'!D5</f>
         <v>6</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="26"/>
       <c r="K6" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L6" s="2">
         <f>SUM(G4:G35)</f>
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="2" t="str">
         <f>'Product backlog'!A6</f>
         <v>HT4</v>
@@ -1638,23 +1695,23 @@
         <f>'Product backlog'!B6</f>
         <v>Configurar los servidores y motores de lenguaje</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="2">
         <f>'Product backlog'!D6</f>
         <v>2</v>
       </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="26"/>
       <c r="K7" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L7" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="2" t="str">
         <f>'Product backlog'!A7</f>
         <v>HT5</v>
@@ -1663,24 +1720,24 @@
         <f>'Product backlog'!B7</f>
         <v>Configurar repositorio GitHub</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
       <c r="G8" s="2">
         <f>'Product backlog'!D7</f>
         <v>1</v>
       </c>
-      <c r="H8" s="21"/>
+      <c r="H8" s="26"/>
       <c r="K8" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L8" s="2">
         <f>L6/L7</f>
-        <v>9.5</v>
+        <v>9.9166666666666661</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="21"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="2" t="str">
         <f>'Product backlog'!A8</f>
         <v>HT6</v>
@@ -1689,113 +1746,112 @@
         <f>'Product backlog'!B8</f>
         <v>Implementar la base de datos</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
       <c r="G9" s="2">
         <f>'Product backlog'!D8</f>
         <v>1</v>
       </c>
-      <c r="H9" s="21"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="14">
+      <c r="A10" s="17">
         <v>2</v>
       </c>
-      <c r="B10" s="2" t="str">
+      <c r="B10" s="36" t="str">
         <f>'Product backlog'!A9</f>
         <v>HT7</v>
       </c>
-      <c r="C10" s="2" t="str">
+      <c r="C10" s="36" t="str">
         <f>'Product backlog'!B9</f>
         <v>Establecer el diseño de las interfaces</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="16">
+      <c r="D10" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="38">
         <v>45363</v>
       </c>
-      <c r="F10" s="14">
-        <v>6</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F10" s="37">
+        <v>6</v>
+      </c>
+      <c r="G10" s="39">
         <f>'Product backlog'!D9</f>
         <v>6</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="37">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="15"/>
-      <c r="B11" s="2" t="str">
+      <c r="A11" s="18"/>
+      <c r="B11" s="36" t="str">
         <f>'Product backlog'!A10</f>
         <v>HT8</v>
       </c>
-      <c r="C11" s="2" t="str">
+      <c r="C11" s="36" t="str">
         <f>'Product backlog'!B10</f>
         <v>Aprendizaje del framework FastAPI y React</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="3">
+      <c r="D11" s="40"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="39">
         <f>'Product backlog'!D10</f>
         <v>6</v>
       </c>
-      <c r="H11" s="15"/>
+      <c r="H11" s="40"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="14">
+      <c r="A12" s="21">
         <v>3</v>
       </c>
-      <c r="B12" s="3" t="str">
+      <c r="B12" s="11" t="str">
         <f>'Product backlog'!A11</f>
         <v>HU1</v>
       </c>
-      <c r="C12" s="3" t="str">
+      <c r="C12" s="11" t="str">
         <f>'Product backlog'!B11</f>
         <v>Visualizar la página principal</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="27">
         <v>45363</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="27">
         <v>45577</v>
       </c>
-      <c r="F12" s="14">
-        <v>6</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="F12" s="21">
+        <v>6</v>
+      </c>
+      <c r="G12" s="11">
         <f>'Product backlog'!D11</f>
         <v>3</v>
       </c>
-      <c r="H12" s="14">
-        <v>7</v>
+      <c r="H12" s="21">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="15"/>
-      <c r="B13" s="3" t="str">
+      <c r="A13" s="22"/>
+      <c r="B13" s="11" t="str">
         <f>'Product backlog'!A12</f>
         <v>HU2</v>
       </c>
-      <c r="C13" s="3" t="str">
+      <c r="C13" s="11" t="str">
         <f>'Product backlog'!B12</f>
-        <v>Registrar cliente</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="3">
-        <f>'Product backlog'!D12</f>
-        <v>4</v>
-      </c>
-      <c r="H13" s="15"/>
+        <v>Gestionar registro y autenticacion de usuarios</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="11">
+        <v>9</v>
+      </c>
+      <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="14">
+      <c r="A14" s="17">
         <v>4</v>
       </c>
       <c r="B14" s="3" t="str">
@@ -1804,27 +1860,27 @@
       </c>
       <c r="C14" s="3" t="str">
         <f>'Product backlog'!B13</f>
-        <v>Autenticar usuario</v>
-      </c>
-      <c r="D14" s="16">
+        <v>Visualizar panel de inicio</v>
+      </c>
+      <c r="D14" s="19">
         <v>45577</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="14">
+      <c r="E14" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="17">
         <v>6</v>
       </c>
       <c r="G14" s="3">
         <f>'Product backlog'!D13</f>
-        <v>4</v>
-      </c>
-      <c r="H14" s="14">
+        <v>2</v>
+      </c>
+      <c r="H14" s="17">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="15"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="3" t="str">
         <f>'Product backlog'!A14</f>
         <v>HU5</v>
@@ -1833,17 +1889,17 @@
         <f>'Product backlog'!B14</f>
         <v>Gestionar membresías</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="15"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="18"/>
       <c r="G15" s="3">
         <f>'Product backlog'!D14</f>
-        <v>6</v>
-      </c>
-      <c r="H15" s="15"/>
+        <v>8</v>
+      </c>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="14">
+      <c r="A16" s="17">
         <v>5</v>
       </c>
       <c r="B16" s="3" t="str">
@@ -1854,25 +1910,25 @@
         <f>'Product backlog'!B15</f>
         <v>Visualizar membresías disponibles</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="14">
+      <c r="D16" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="17">
         <v>6</v>
       </c>
       <c r="G16" s="3">
         <f>'Product backlog'!D15</f>
         <v>2</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="17">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="15"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="3" t="str">
         <f>'Product backlog'!A16</f>
         <v>HU7</v>
@@ -1881,17 +1937,17 @@
         <f>'Product backlog'!B16</f>
         <v>Comprar membresía</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="15"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="18"/>
       <c r="G17" s="3">
         <f>'Product backlog'!D16</f>
         <v>6</v>
       </c>
-      <c r="H17" s="15"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="14">
+      <c r="A18" s="17">
         <v>6</v>
       </c>
       <c r="B18" s="3" t="str">
@@ -1902,25 +1958,25 @@
         <f>'Product backlog'!B17</f>
         <v>Visualizar y Modificar sueldo Básico</v>
       </c>
-      <c r="D18" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="14">
+      <c r="D18" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="17">
         <v>6</v>
       </c>
       <c r="G18" s="3">
         <f>'Product backlog'!D17</f>
         <v>1</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="17">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="22"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="3" t="str">
         <f>'Product backlog'!A18</f>
         <v>HU21</v>
@@ -1929,17 +1985,17 @@
         <f>'Product backlog'!B18</f>
         <v>Gestionar categorías de gastos</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="22"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="29"/>
       <c r="G19" s="3">
         <f>'Product backlog'!D18</f>
         <v>5</v>
       </c>
-      <c r="H19" s="22"/>
+      <c r="H19" s="29"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="15"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="3" t="str">
         <f>'Product backlog'!A19</f>
         <v>HU9</v>
@@ -1948,17 +2004,17 @@
         <f>'Product backlog'!B19</f>
         <v>Extraer comprobantes electrónicos</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="15"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="18"/>
       <c r="G20" s="3">
         <f>'Product backlog'!D19</f>
         <v>5</v>
       </c>
-      <c r="H20" s="15"/>
+      <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="14">
+      <c r="A21" s="17">
         <v>7</v>
       </c>
       <c r="B21" s="3" t="str">
@@ -1969,25 +2025,25 @@
         <f>'Product backlog'!B20</f>
         <v>Carga de comprobantes electrónicos</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="16">
+      <c r="D21" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="19">
         <v>45839</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="17">
         <v>6</v>
       </c>
       <c r="G21" s="3">
         <f>'Product backlog'!D20</f>
         <v>4</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="17">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="15"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="3" t="str">
         <f>'Product backlog'!A21</f>
         <v>HU11</v>
@@ -1996,17 +2052,17 @@
         <f>'Product backlog'!B21</f>
         <v>Listar comprobantes cargados</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="15"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="18"/>
       <c r="G22" s="3">
         <f>'Product backlog'!D21</f>
         <v>3</v>
       </c>
-      <c r="H22" s="15"/>
+      <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="14">
+      <c r="A23" s="17">
         <v>8</v>
       </c>
       <c r="B23" s="3" t="str">
@@ -2017,25 +2073,25 @@
         <f>'Product backlog'!B22</f>
         <v>Asignar categoría al comprobante</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="19">
         <v>45839</v>
       </c>
-      <c r="E23" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="14">
+      <c r="E23" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="17">
         <v>6</v>
       </c>
       <c r="G23" s="3">
         <f>'Product backlog'!D22</f>
         <v>2</v>
       </c>
-      <c r="H23" s="14">
+      <c r="H23" s="17">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="22"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="3" t="str">
         <f>'Product backlog'!A23</f>
         <v>HU14</v>
@@ -2044,17 +2100,17 @@
         <f>'Product backlog'!B23</f>
         <v>Generar documento deducción de impuestos</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
       <c r="G24" s="3">
         <f>'Product backlog'!D23</f>
         <v>5</v>
       </c>
-      <c r="H24" s="22"/>
+      <c r="H24" s="29"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="15"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="3" t="str">
         <f>'Product backlog'!A24</f>
         <v>HU18</v>
@@ -2063,17 +2119,17 @@
         <f>'Product backlog'!B24</f>
         <v>Visualizar y modificar datos del administrador</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
       <c r="G25" s="3">
         <f>'Product backlog'!D24</f>
         <v>2</v>
       </c>
-      <c r="H25" s="15"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="14">
+      <c r="A26" s="17">
         <v>9</v>
       </c>
       <c r="B26" s="3" t="str">
@@ -2084,25 +2140,25 @@
         <f>'Product backlog'!B25</f>
         <v>Implementar el modelo de machine learning</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="F26" s="14">
+      <c r="D26" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="17">
         <v>6</v>
       </c>
       <c r="G26" s="3">
         <f>'Product backlog'!D25</f>
         <v>6</v>
       </c>
-      <c r="H26" s="14">
+      <c r="H26" s="17">
         <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="15"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="3" t="str">
         <f>'Product backlog'!A26</f>
         <v>HU17</v>
@@ -2111,17 +2167,17 @@
         <f>'Product backlog'!B26</f>
         <v>Visualizar predicción de gastos</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
       <c r="G27" s="3">
         <f>'Product backlog'!D26</f>
         <v>6</v>
       </c>
-      <c r="H27" s="15"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="14">
+      <c r="A28" s="17">
         <v>10</v>
       </c>
       <c r="B28" s="3" t="str">
@@ -2132,25 +2188,25 @@
         <f>'Product backlog'!B27</f>
         <v>Visualizar comprobante específico</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F28" s="14">
+      <c r="D28" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="17">
         <v>5</v>
       </c>
       <c r="G28" s="3">
         <f>'Product backlog'!D27</f>
         <v>2</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="17">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="22"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="3" t="str">
         <f>'Product backlog'!A28</f>
         <v>HU8</v>
@@ -2159,17 +2215,17 @@
         <f>'Product backlog'!B28</f>
         <v>Visualizar estado de la membresía adquirida</v>
       </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
       <c r="G29" s="3">
         <f>'Product backlog'!D28</f>
         <v>2</v>
       </c>
-      <c r="H29" s="22"/>
+      <c r="H29" s="29"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="15"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="3" t="str">
         <f>'Product backlog'!A29</f>
         <v>HU4</v>
@@ -2178,17 +2234,17 @@
         <f>'Product backlog'!B29</f>
         <v>Visualizar y modificar datos del usuario</v>
       </c>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
       <c r="G30" s="3">
         <f>'Product backlog'!D29</f>
         <v>3</v>
       </c>
-      <c r="H30" s="15"/>
+      <c r="H30" s="18"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="14">
+      <c r="A31" s="17">
         <v>11</v>
       </c>
       <c r="B31" s="3" t="str">
@@ -2199,25 +2255,25 @@
         <f>'Product backlog'!B30</f>
         <v>Visualizar historial de deducciones</v>
       </c>
-      <c r="D31" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="16">
+      <c r="D31" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="19">
         <v>45749</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="17">
         <v>6</v>
       </c>
       <c r="G31" s="3">
         <f>'Product backlog'!D30</f>
         <v>2</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="17">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="22"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="3" t="str">
         <f>'Product backlog'!A31</f>
         <v>HU19</v>
@@ -2226,17 +2282,17 @@
         <f>'Product backlog'!B31</f>
         <v>Listar clientes registrados</v>
       </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="22"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="29"/>
       <c r="G32" s="3">
         <f>'Product backlog'!D31</f>
         <v>2</v>
       </c>
-      <c r="H32" s="22"/>
+      <c r="H32" s="29"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="15"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="3" t="str">
         <f>'Product backlog'!A32</f>
         <v>HU16</v>
@@ -2245,17 +2301,17 @@
         <f>'Product backlog'!B32</f>
         <v>Darse de baja del sistema</v>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="15"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="18"/>
       <c r="G33" s="3">
         <f>'Product backlog'!D32</f>
         <v>3</v>
       </c>
-      <c r="H33" s="15"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="14">
+      <c r="A34" s="17">
         <v>12</v>
       </c>
       <c r="B34" s="5" t="str">
@@ -2266,25 +2322,25 @@
         <f>'Product backlog'!B33</f>
         <v>Refactorización del código</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="19">
         <v>45748</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="19">
         <v>45901</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="17">
         <v>5</v>
       </c>
       <c r="G34" s="4">
         <f>'Product backlog'!D33</f>
         <v>6</v>
       </c>
-      <c r="H34" s="14">
+      <c r="H34" s="17">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="15"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="5" t="str">
         <f>'Product backlog'!A34</f>
         <v>HT11</v>
@@ -2293,14 +2349,14 @@
         <f>'Product backlog'!B34</f>
         <v>Despliegue y puesta a punto</v>
       </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="15"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="18"/>
       <c r="G35" s="4">
         <f>'Product backlog'!D34</f>
         <v>6</v>
       </c>
-      <c r="H35" s="15"/>
+      <c r="H35" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="65">

</xml_diff>

<commit_message>
requisitos de reestableces y actualizar contrasenia
</commit_message>
<xml_diff>
--- a/documentacion/scrum/Product backlog.xlsx
+++ b/documentacion/scrum/Product backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyecto\documentacion\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FCB278-DA70-41AD-8576-7ACC547B1480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688920FA-B8F2-42EA-8EB2-698916A97D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{62494E98-7055-48D3-B966-884A22B78DF5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sprint backlog" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc182169169" localSheetId="1">'Product backlog'!$F$2</definedName>
+    <definedName name="_Toc182169169" localSheetId="1">'Product backlog'!$G$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="113">
   <si>
     <t>Product backlog</t>
   </si>
@@ -361,6 +361,24 @@
   </si>
   <si>
     <t>Visualizar panel de inicio</t>
+  </si>
+  <si>
+    <t>HU22</t>
+  </si>
+  <si>
+    <t>Requisitos</t>
+  </si>
+  <si>
+    <t>Ver detalles y descargar Documento de Deducción</t>
+  </si>
+  <si>
+    <t>RF26, RF27</t>
+  </si>
+  <si>
+    <t>Reestablecer y actualizar contraseña</t>
+  </si>
+  <si>
+    <t>HU23</t>
   </si>
 </sst>
 </file>
@@ -529,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -556,6 +574,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,24 +606,36 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -622,24 +657,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,32 +998,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A306DB25-FA75-4E4E-8913-B4C3461E94DB}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="39.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="8" max="8" width="11.6328125" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" customWidth="1"/>
-    <col min="10" max="10" width="43.453125" customWidth="1"/>
+    <col min="2" max="2" width="42.36328125" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="8.6328125" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="11.6328125" customWidth="1"/>
+    <col min="10" max="10" width="13.36328125" customWidth="1"/>
+    <col min="11" max="11" width="43.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1007,532 +1033,599 @@
         <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="2">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>2</v>
       </c>
-      <c r="F6" s="34">
+      <c r="G6" s="12">
         <v>45394</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>3</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J6" s="35" t="s">
+      <c r="K6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E9" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E10" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E14" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E15" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E16" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="E17" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E18" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E19" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E20" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="2">
+      <c r="E21" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="2">
+      <c r="E22" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="2">
+      <c r="E23" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="2">
+      <c r="E24" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="2">
+      <c r="E26" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+      <c r="E27" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="E28" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="2">
+      <c r="E29" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="2">
+      <c r="E30" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="2">
+      <c r="E31" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="2">
+      <c r="E32" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="2">
+      <c r="E33" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="2">
+      <c r="E34" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
+      <c r="E35" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="2">
+      <c r="E36" s="2">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G2:K2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1542,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49D8E50-E16B-43C7-A737-D72E991DFD2E}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1562,39 +1655,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="8" t="s">
         <v>71</v>
       </c>
@@ -1612,7 +1705,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+      <c r="A4" s="29">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="str">
@@ -1623,25 +1716,25 @@
         <f>'Product backlog'!B3</f>
         <v>Instalar las herramientas de desarrollo</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="29">
         <v>6</v>
       </c>
       <c r="G4" s="2">
-        <f>'Product backlog'!D3</f>
+        <f>'Product backlog'!E3</f>
         <v>1</v>
       </c>
-      <c r="H4" s="26">
+      <c r="H4" s="29">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="26"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="2" t="str">
         <f>'Product backlog'!A4</f>
         <v>HT2</v>
@@ -1650,17 +1743,17 @@
         <f>'Product backlog'!B4</f>
         <v>Establecer el estándar de codificación</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="2">
-        <f>'Product backlog'!D4</f>
+        <f>'Product backlog'!E4</f>
         <v>1</v>
       </c>
-      <c r="H5" s="26"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="26"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="2" t="str">
         <f>'Product backlog'!A5</f>
         <v>HT3</v>
@@ -1669,24 +1762,24 @@
         <f>'Product backlog'!B5</f>
         <v>Establecer el diseño de base de datos</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
       <c r="G6" s="2">
-        <f>'Product backlog'!D5</f>
-        <v>6</v>
-      </c>
-      <c r="H6" s="26"/>
+        <f>'Product backlog'!E5</f>
+        <v>6</v>
+      </c>
+      <c r="H6" s="29"/>
       <c r="K6" s="2" t="s">
         <v>87</v>
       </c>
       <c r="L6" s="2">
-        <f>SUM(G4:G35)</f>
-        <v>119</v>
+        <f>SUM(G4:G37)</f>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="26"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2" t="str">
         <f>'Product backlog'!A6</f>
         <v>HT4</v>
@@ -1695,14 +1788,14 @@
         <f>'Product backlog'!B6</f>
         <v>Configurar los servidores y motores de lenguaje</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
       <c r="G7" s="2">
-        <f>'Product backlog'!D6</f>
+        <f>'Product backlog'!E6</f>
         <v>2</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="29"/>
       <c r="K7" s="2" t="s">
         <v>77</v>
       </c>
@@ -1711,7 +1804,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="26"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="2" t="str">
         <f>'Product backlog'!A7</f>
         <v>HT5</v>
@@ -1720,24 +1813,24 @@
         <f>'Product backlog'!B7</f>
         <v>Configurar repositorio GitHub</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="2">
-        <f>'Product backlog'!D7</f>
+        <f>'Product backlog'!E7</f>
         <v>1</v>
       </c>
-      <c r="H8" s="26"/>
+      <c r="H8" s="29"/>
       <c r="K8" s="2" t="s">
         <v>78</v>
       </c>
       <c r="L8" s="2">
         <f>L6/L7</f>
-        <v>9.9166666666666661</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="26"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="2" t="str">
         <f>'Product backlog'!A8</f>
         <v>HT6</v>
@@ -1746,669 +1839,707 @@
         <f>'Product backlog'!B8</f>
         <v>Implementar la base de datos</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="2">
-        <f>'Product backlog'!D8</f>
+        <f>'Product backlog'!E8</f>
         <v>1</v>
       </c>
-      <c r="H9" s="26"/>
+      <c r="H9" s="29"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="17">
+      <c r="A10" s="20">
         <v>2</v>
       </c>
-      <c r="B10" s="36" t="str">
+      <c r="B10" s="13" t="str">
         <f>'Product backlog'!A9</f>
         <v>HT7</v>
       </c>
-      <c r="C10" s="36" t="str">
+      <c r="C10" s="13" t="str">
         <f>'Product backlog'!B9</f>
         <v>Establecer el diseño de las interfaces</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="30">
         <v>45363</v>
       </c>
-      <c r="F10" s="37">
-        <v>6</v>
-      </c>
-      <c r="G10" s="39">
-        <f>'Product backlog'!D9</f>
-        <v>6</v>
-      </c>
-      <c r="H10" s="37">
+      <c r="F10" s="24">
+        <v>6</v>
+      </c>
+      <c r="G10" s="14">
+        <f>'Product backlog'!E9</f>
+        <v>6</v>
+      </c>
+      <c r="H10" s="24">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="18"/>
-      <c r="B11" s="36" t="str">
+      <c r="A11" s="21"/>
+      <c r="B11" s="13" t="str">
         <f>'Product backlog'!A10</f>
         <v>HT8</v>
       </c>
-      <c r="C11" s="36" t="str">
+      <c r="C11" s="13" t="str">
         <f>'Product backlog'!B10</f>
         <v>Aprendizaje del framework FastAPI y React</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="39">
-        <f>'Product backlog'!D10</f>
-        <v>6</v>
-      </c>
-      <c r="H11" s="40"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="14">
+        <f>'Product backlog'!E10</f>
+        <v>6</v>
+      </c>
+      <c r="H11" s="25"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="21">
+      <c r="A12" s="20">
         <v>3</v>
       </c>
-      <c r="B12" s="11" t="str">
+      <c r="B12" s="3" t="str">
         <f>'Product backlog'!A11</f>
         <v>HU1</v>
       </c>
-      <c r="C12" s="11" t="str">
+      <c r="C12" s="3" t="str">
         <f>'Product backlog'!B11</f>
         <v>Visualizar la página principal</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="22">
         <v>45363</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="22">
         <v>45577</v>
       </c>
-      <c r="F12" s="21">
-        <v>6</v>
-      </c>
-      <c r="G12" s="11">
-        <f>'Product backlog'!D11</f>
+      <c r="F12" s="20">
+        <v>6</v>
+      </c>
+      <c r="G12" s="3">
+        <f>'Product backlog'!E11</f>
         <v>3</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="20">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="22"/>
-      <c r="B13" s="11" t="str">
+      <c r="A13" s="21"/>
+      <c r="B13" s="3" t="str">
         <f>'Product backlog'!A12</f>
         <v>HU2</v>
       </c>
-      <c r="C13" s="11" t="str">
+      <c r="C13" s="3" t="str">
         <f>'Product backlog'!B12</f>
         <v>Gestionar registro y autenticacion de usuarios</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="11">
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="3">
         <v>9</v>
       </c>
-      <c r="H13" s="22"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="17">
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="1:12" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="32">
         <v>4</v>
       </c>
-      <c r="B14" s="3" t="str">
+      <c r="B14" s="11" t="str">
         <f>'Product backlog'!A13</f>
+        <v>HU23</v>
+      </c>
+      <c r="C14" s="11" t="str">
+        <f>'Product backlog'!B13</f>
+        <v>Reestablecer y actualizar contraseña</v>
+      </c>
+      <c r="D14" s="34">
+        <v>45577</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="32">
+        <v>6</v>
+      </c>
+      <c r="G14" s="11">
+        <f>'Product backlog'!E13</f>
+        <v>4</v>
+      </c>
+      <c r="H14" s="32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="41"/>
+      <c r="B15" s="11" t="str">
+        <f>'Product backlog'!A14</f>
         <v>HU3</v>
       </c>
-      <c r="C14" s="3" t="str">
-        <f>'Product backlog'!B13</f>
+      <c r="C15" s="11" t="str">
+        <f>'Product backlog'!B14</f>
         <v>Visualizar panel de inicio</v>
       </c>
-      <c r="D14" s="19">
-        <v>45577</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="17">
-        <v>6</v>
-      </c>
-      <c r="G14" s="3">
-        <f>'Product backlog'!D13</f>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="11">
+        <f>'Product backlog'!E14</f>
         <v>2</v>
       </c>
-      <c r="H14" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="18"/>
-      <c r="B15" s="3" t="str">
-        <f>'Product backlog'!A14</f>
+      <c r="H15" s="41"/>
+    </row>
+    <row r="16" spans="1:12" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="33"/>
+      <c r="B16" s="11" t="str">
+        <f>'Product backlog'!A15</f>
         <v>HU5</v>
       </c>
-      <c r="C15" s="3" t="str">
-        <f>'Product backlog'!B14</f>
+      <c r="C16" s="11" t="str">
+        <f>'Product backlog'!B15</f>
         <v>Gestionar membresías</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="3">
-        <f>'Product backlog'!D14</f>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="11">
+        <f>'Product backlog'!E15</f>
         <v>8</v>
       </c>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="17">
+      <c r="H16" s="33"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="20">
         <v>5</v>
       </c>
-      <c r="B16" s="3" t="str">
-        <f>'Product backlog'!A15</f>
-        <v>HU6</v>
-      </c>
-      <c r="C16" s="3" t="str">
-        <f>'Product backlog'!B15</f>
-        <v>Visualizar membresías disponibles</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16" s="17">
-        <v>6</v>
-      </c>
-      <c r="G16" s="3">
-        <f>'Product backlog'!D15</f>
-        <v>2</v>
-      </c>
-      <c r="H16" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="18"/>
       <c r="B17" s="3" t="str">
         <f>'Product backlog'!A16</f>
-        <v>HU7</v>
+        <v>HU6</v>
       </c>
       <c r="C17" s="3" t="str">
         <f>'Product backlog'!B16</f>
-        <v>Comprar membresía</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="18"/>
+        <v>Visualizar membresías disponibles</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="20">
+        <v>6</v>
+      </c>
       <c r="G17" s="3">
-        <f>'Product backlog'!D16</f>
-        <v>6</v>
-      </c>
-      <c r="H17" s="18"/>
+        <f>'Product backlog'!E16</f>
+        <v>2</v>
+      </c>
+      <c r="H17" s="20">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="17">
-        <v>6</v>
-      </c>
+      <c r="A18" s="21"/>
       <c r="B18" s="3" t="str">
         <f>'Product backlog'!A17</f>
-        <v>HU20</v>
+        <v>HU7</v>
       </c>
       <c r="C18" s="3" t="str">
         <f>'Product backlog'!B17</f>
-        <v>Visualizar y Modificar sueldo Básico</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="17">
-        <v>6</v>
-      </c>
+        <v>Comprar membresía</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="3">
-        <f>'Product backlog'!D17</f>
-        <v>1</v>
-      </c>
-      <c r="H18" s="17">
-        <v>11</v>
-      </c>
+        <f>'Product backlog'!E17</f>
+        <v>6</v>
+      </c>
+      <c r="H18" s="21"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="29"/>
+      <c r="A19" s="20">
+        <v>6</v>
+      </c>
       <c r="B19" s="3" t="str">
         <f>'Product backlog'!A18</f>
-        <v>HU21</v>
+        <v>HU20</v>
       </c>
       <c r="C19" s="3" t="str">
         <f>'Product backlog'!B18</f>
-        <v>Gestionar categorías de gastos</v>
-      </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="29"/>
+        <v>Visualizar y Modificar sueldo Básico</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="20">
+        <v>6</v>
+      </c>
       <c r="G19" s="3">
-        <f>'Product backlog'!D18</f>
-        <v>5</v>
-      </c>
-      <c r="H19" s="29"/>
+        <f>'Product backlog'!E18</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="20">
+        <v>11</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="18"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="3" t="str">
         <f>'Product backlog'!A19</f>
-        <v>HU9</v>
+        <v>HU21</v>
       </c>
       <c r="C20" s="3" t="str">
         <f>'Product backlog'!B19</f>
-        <v>Extraer comprobantes electrónicos</v>
-      </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="18"/>
+        <v>Gestionar categorías de gastos</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="36"/>
       <c r="G20" s="3">
-        <f>'Product backlog'!D19</f>
+        <f>'Product backlog'!E19</f>
         <v>5</v>
       </c>
-      <c r="H20" s="18"/>
+      <c r="H20" s="36"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="17">
-        <v>7</v>
-      </c>
+      <c r="A21" s="21"/>
       <c r="B21" s="3" t="str">
         <f>'Product backlog'!A20</f>
-        <v>HU10</v>
+        <v>HU9</v>
       </c>
       <c r="C21" s="3" t="str">
         <f>'Product backlog'!B20</f>
-        <v>Carga de comprobantes electrónicos</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="19">
-        <v>45839</v>
-      </c>
-      <c r="F21" s="17">
-        <v>6</v>
-      </c>
+        <v>Extraer comprobantes electrónicos</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="21"/>
       <c r="G21" s="3">
-        <f>'Product backlog'!D20</f>
-        <v>4</v>
-      </c>
-      <c r="H21" s="17">
+        <f>'Product backlog'!E20</f>
+        <v>5</v>
+      </c>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="20">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="18"/>
       <c r="B22" s="3" t="str">
         <f>'Product backlog'!A21</f>
-        <v>HU11</v>
+        <v>HU10</v>
       </c>
       <c r="C22" s="3" t="str">
         <f>'Product backlog'!B21</f>
-        <v>Listar comprobantes cargados</v>
-      </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="18"/>
+        <v>Carga de comprobantes electrónicos</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="22">
+        <v>45839</v>
+      </c>
+      <c r="F22" s="20">
+        <v>6</v>
+      </c>
       <c r="G22" s="3">
-        <f>'Product backlog'!D21</f>
-        <v>3</v>
-      </c>
-      <c r="H22" s="18"/>
+        <f>'Product backlog'!E21</f>
+        <v>4</v>
+      </c>
+      <c r="H22" s="20">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="17">
-        <v>8</v>
-      </c>
+      <c r="A23" s="21"/>
       <c r="B23" s="3" t="str">
         <f>'Product backlog'!A22</f>
-        <v>HU12</v>
+        <v>HU11</v>
       </c>
       <c r="C23" s="3" t="str">
         <f>'Product backlog'!B22</f>
-        <v>Asignar categoría al comprobante</v>
-      </c>
-      <c r="D23" s="19">
-        <v>45839</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" s="17">
-        <v>6</v>
-      </c>
+        <v>Listar comprobantes cargados</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="3">
-        <f>'Product backlog'!D22</f>
-        <v>2</v>
-      </c>
-      <c r="H23" s="17">
-        <v>9</v>
-      </c>
+        <f>'Product backlog'!E22</f>
+        <v>3</v>
+      </c>
+      <c r="H23" s="21"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="29"/>
+      <c r="A24" s="20">
+        <v>8</v>
+      </c>
       <c r="B24" s="3" t="str">
         <f>'Product backlog'!A23</f>
-        <v>HU14</v>
+        <v>HU12</v>
       </c>
       <c r="C24" s="3" t="str">
         <f>'Product backlog'!B23</f>
-        <v>Generar documento deducción de impuestos</v>
-      </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
+        <v>Asignar categoría al comprobante</v>
+      </c>
+      <c r="D24" s="22">
+        <v>45839</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="20">
+        <v>6</v>
+      </c>
       <c r="G24" s="3">
-        <f>'Product backlog'!D23</f>
-        <v>5</v>
-      </c>
-      <c r="H24" s="29"/>
+        <f>'Product backlog'!E23</f>
+        <v>2</v>
+      </c>
+      <c r="H24" s="20">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="18"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="3" t="str">
         <f>'Product backlog'!A24</f>
-        <v>HU18</v>
+        <v>HU14</v>
       </c>
       <c r="C25" s="3" t="str">
         <f>'Product backlog'!B24</f>
-        <v>Visualizar y modificar datos del administrador</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
+        <v>Generar documento deducción de impuestos</v>
+      </c>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
       <c r="G25" s="3">
-        <f>'Product backlog'!D24</f>
-        <v>2</v>
-      </c>
-      <c r="H25" s="18"/>
+        <f>'Product backlog'!E24</f>
+        <v>5</v>
+      </c>
+      <c r="H25" s="36"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="17">
-        <v>9</v>
-      </c>
+      <c r="A26" s="36"/>
       <c r="B26" s="3" t="str">
         <f>'Product backlog'!A25</f>
-        <v>HT9</v>
+        <v>HU22</v>
       </c>
       <c r="C26" s="3" t="str">
         <f>'Product backlog'!B25</f>
-        <v>Implementar el modelo de machine learning</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" s="17">
-        <v>6</v>
-      </c>
+        <v>Ver detalles y descargar Documento de Deducción</v>
+      </c>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="3">
-        <f>'Product backlog'!D25</f>
-        <v>6</v>
-      </c>
-      <c r="H26" s="17">
-        <v>12</v>
-      </c>
+        <f>'Product backlog'!E25</f>
+        <v>6</v>
+      </c>
+      <c r="H26" s="36"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="18"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="3" t="str">
         <f>'Product backlog'!A26</f>
-        <v>HU17</v>
+        <v>HU18</v>
       </c>
       <c r="C27" s="3" t="str">
         <f>'Product backlog'!B26</f>
-        <v>Visualizar predicción de gastos</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
+        <v>Visualizar y modificar datos del administrador</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="3">
-        <f>'Product backlog'!D26</f>
-        <v>6</v>
-      </c>
-      <c r="H27" s="18"/>
+        <f>'Product backlog'!E26</f>
+        <v>2</v>
+      </c>
+      <c r="H27" s="21"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="17">
-        <v>10</v>
+      <c r="A28" s="20">
+        <v>9</v>
       </c>
       <c r="B28" s="3" t="str">
         <f>'Product backlog'!A27</f>
-        <v>HU13</v>
+        <v>HT9</v>
       </c>
       <c r="C28" s="3" t="str">
         <f>'Product backlog'!B27</f>
-        <v>Visualizar comprobante específico</v>
-      </c>
-      <c r="D28" s="17" t="s">
+        <v>Implementar el modelo de machine learning</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E28" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F28" s="17">
-        <v>5</v>
+      <c r="F28" s="20">
+        <v>6</v>
       </c>
       <c r="G28" s="3">
-        <f>'Product backlog'!D27</f>
-        <v>2</v>
-      </c>
-      <c r="H28" s="17">
-        <v>7</v>
+        <f>'Product backlog'!E27</f>
+        <v>6</v>
+      </c>
+      <c r="H28" s="20">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="29"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="3" t="str">
         <f>'Product backlog'!A28</f>
-        <v>HU8</v>
+        <v>HU17</v>
       </c>
       <c r="C29" s="3" t="str">
         <f>'Product backlog'!B28</f>
-        <v>Visualizar estado de la membresía adquirida</v>
-      </c>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
+        <v>Visualizar predicción de gastos</v>
+      </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
       <c r="G29" s="3">
-        <f>'Product backlog'!D28</f>
-        <v>2</v>
-      </c>
-      <c r="H29" s="29"/>
+        <f>'Product backlog'!E28</f>
+        <v>6</v>
+      </c>
+      <c r="H29" s="21"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="18"/>
+      <c r="A30" s="20">
+        <v>10</v>
+      </c>
       <c r="B30" s="3" t="str">
         <f>'Product backlog'!A29</f>
-        <v>HU4</v>
+        <v>HU13</v>
       </c>
       <c r="C30" s="3" t="str">
         <f>'Product backlog'!B29</f>
-        <v>Visualizar y modificar datos del usuario</v>
-      </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
+        <v>Visualizar comprobante específico</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="20">
+        <v>5</v>
+      </c>
       <c r="G30" s="3">
-        <f>'Product backlog'!D29</f>
-        <v>3</v>
-      </c>
-      <c r="H30" s="18"/>
+        <f>'Product backlog'!E29</f>
+        <v>2</v>
+      </c>
+      <c r="H30" s="20">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="17">
-        <v>11</v>
-      </c>
+      <c r="A31" s="36"/>
       <c r="B31" s="3" t="str">
         <f>'Product backlog'!A30</f>
-        <v>HU15</v>
+        <v>HU8</v>
       </c>
       <c r="C31" s="3" t="str">
         <f>'Product backlog'!B30</f>
-        <v>Visualizar historial de deducciones</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" s="19">
-        <v>45749</v>
-      </c>
-      <c r="F31" s="17">
-        <v>6</v>
-      </c>
+        <v>Visualizar estado de la membresía adquirida</v>
+      </c>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
       <c r="G31" s="3">
-        <f>'Product backlog'!D30</f>
+        <f>'Product backlog'!E30</f>
         <v>2</v>
       </c>
-      <c r="H31" s="17">
-        <v>7</v>
-      </c>
+      <c r="H31" s="36"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="29"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="3" t="str">
         <f>'Product backlog'!A31</f>
-        <v>HU19</v>
+        <v>HU4</v>
       </c>
       <c r="C32" s="3" t="str">
         <f>'Product backlog'!B31</f>
-        <v>Listar clientes registrados</v>
-      </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="29"/>
+        <v>Visualizar y modificar datos del usuario</v>
+      </c>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="3">
-        <f>'Product backlog'!D31</f>
-        <v>2</v>
-      </c>
-      <c r="H32" s="29"/>
+        <f>'Product backlog'!E31</f>
+        <v>3</v>
+      </c>
+      <c r="H32" s="21"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="18"/>
+      <c r="A33" s="20">
+        <v>11</v>
+      </c>
       <c r="B33" s="3" t="str">
         <f>'Product backlog'!A32</f>
-        <v>HU16</v>
+        <v>HU15</v>
       </c>
       <c r="C33" s="3" t="str">
         <f>'Product backlog'!B32</f>
-        <v>Darse de baja del sistema</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="18"/>
+        <v>Visualizar historial de deducciones</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="22">
+        <v>45749</v>
+      </c>
+      <c r="F33" s="20">
+        <v>6</v>
+      </c>
       <c r="G33" s="3">
-        <f>'Product backlog'!D32</f>
-        <v>3</v>
-      </c>
-      <c r="H33" s="18"/>
+        <f>'Product backlog'!E32</f>
+        <v>2</v>
+      </c>
+      <c r="H33" s="20">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="17">
-        <v>12</v>
-      </c>
-      <c r="B34" s="5" t="str">
+      <c r="A34" s="36"/>
+      <c r="B34" s="3" t="str">
         <f>'Product backlog'!A33</f>
-        <v>HT10</v>
+        <v>HU19</v>
       </c>
       <c r="C34" s="3" t="str">
         <f>'Product backlog'!B33</f>
+        <v>Listar clientes registrados</v>
+      </c>
+      <c r="D34" s="36"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="3">
+        <f>'Product backlog'!E33</f>
+        <v>2</v>
+      </c>
+      <c r="H34" s="36"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="21"/>
+      <c r="B35" s="3" t="str">
+        <f>'Product backlog'!A34</f>
+        <v>HU16</v>
+      </c>
+      <c r="C35" s="3" t="str">
+        <f>'Product backlog'!B34</f>
+        <v>Darse de baja del sistema</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="3">
+        <f>'Product backlog'!E34</f>
+        <v>3</v>
+      </c>
+      <c r="H35" s="21"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="20">
+        <v>12</v>
+      </c>
+      <c r="B36" s="5" t="str">
+        <f>'Product backlog'!A35</f>
+        <v>HT10</v>
+      </c>
+      <c r="C36" s="3" t="str">
+        <f>'Product backlog'!B35</f>
         <v>Refactorización del código</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D36" s="22">
         <v>45748</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E36" s="22">
         <v>45901</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F36" s="20">
         <v>5</v>
       </c>
-      <c r="G34" s="4">
-        <f>'Product backlog'!D33</f>
-        <v>6</v>
-      </c>
-      <c r="H34" s="17">
+      <c r="G36" s="4">
+        <f>'Product backlog'!E35</f>
+        <v>6</v>
+      </c>
+      <c r="H36" s="20">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="18"/>
-      <c r="B35" s="5" t="str">
-        <f>'Product backlog'!A34</f>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="21"/>
+      <c r="B37" s="5" t="str">
+        <f>'Product backlog'!A36</f>
         <v>HT11</v>
       </c>
-      <c r="C35" s="5" t="str">
-        <f>'Product backlog'!B34</f>
+      <c r="C37" s="5" t="str">
+        <f>'Product backlog'!B36</f>
         <v>Despliegue y puesta a punto</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="4">
-        <f>'Product backlog'!D34</f>
-        <v>6</v>
-      </c>
-      <c r="H35" s="18"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="4">
+        <f>'Product backlog'!E36</f>
+        <v>6</v>
+      </c>
+      <c r="H37" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="H36:H37"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="H30:H32"/>
+    <mergeCell ref="H33:H35"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="F14:F15"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>

</xml_diff>

<commit_message>
correcion historias y arquitectura
</commit_message>
<xml_diff>
--- a/documentacion/scrum/Product backlog.xlsx
+++ b/documentacion/scrum/Product backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyecto\documentacion\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688920FA-B8F2-42EA-8EB2-698916A97D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE1C3FE-AD54-4F09-B71C-C6A435F18019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{62494E98-7055-48D3-B966-884A22B78DF5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{62494E98-7055-48D3-B966-884A22B78DF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="116">
   <si>
     <t>Product backlog</t>
   </si>
@@ -228,9 +228,6 @@
     <t>HU21</t>
   </si>
   <si>
-    <t>Darse de baja del sistema</t>
-  </si>
-  <si>
     <t>Visualizar predicción de gastos</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
     <t xml:space="preserve">Baja   </t>
   </si>
   <si>
-    <t>Visualizar y Modificar sueldo Básico</t>
-  </si>
-  <si>
     <t>Gestionar categorías de gastos</t>
   </si>
   <si>
@@ -339,9 +333,6 @@
     <t>Definición del productk backlog</t>
   </si>
   <si>
-    <t>Sincronización con las historias de usuario y tecnicas</t>
-  </si>
-  <si>
     <t>Aprendizaje del framework FastAPI y React</t>
   </si>
   <si>
@@ -372,13 +363,31 @@
     <t>Ver detalles y descargar Documento de Deducción</t>
   </si>
   <si>
-    <t>RF26, RF27</t>
-  </si>
-  <si>
     <t>Reestablecer y actualizar contraseña</t>
   </si>
   <si>
-    <t>HU23</t>
+    <t>Implementación de JWT</t>
+  </si>
+  <si>
+    <t>HT12</t>
+  </si>
+  <si>
+    <t>Gestionar sueldo Básico</t>
+  </si>
+  <si>
+    <t>HT13</t>
+  </si>
+  <si>
+    <t>Redefinición de las tecnologías del front-end</t>
+  </si>
+  <si>
+    <t>alta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sincronización con las historias de usuario y técnicas </t>
+  </si>
+  <si>
+    <t>Añadir historias técnicas de JWT y Tailwind</t>
   </si>
 </sst>
 </file>
@@ -408,7 +417,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,6 +451,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -555,9 +570,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -574,9 +586,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -630,22 +644,22 @@
     <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -663,7 +677,30 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,57 +1035,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A306DB25-FA75-4E4E-8913-B4C3461E94DB}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="42.36328125" customWidth="1"/>
+    <col min="2" max="2" width="42.453125" customWidth="1"/>
     <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.1796875" customWidth="1"/>
-    <col min="9" max="9" width="11.6328125" customWidth="1"/>
-    <col min="10" max="10" width="13.36328125" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" customWidth="1"/>
     <col min="11" max="11" width="43.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>73</v>
+      <c r="E2" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
+      <c r="G2" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1064,19 +1101,19 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1095,19 +1132,19 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H4" s="2">
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1124,20 +1161,20 @@
       <c r="E5" s="2">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>96</v>
+      <c r="G5" s="48" t="s">
+        <v>94</v>
       </c>
       <c r="H5" s="2">
         <v>2</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1154,20 +1191,20 @@
       <c r="E6" s="2">
         <v>2</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="49">
         <v>45394</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="K6" t="s">
-        <v>104</v>
+        <v>93</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1184,6 +1221,21 @@
       <c r="E7" s="2">
         <v>1</v>
       </c>
+      <c r="G7" s="49">
+        <v>45809</v>
+      </c>
+      <c r="H7" s="2">
+        <v>4</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -1199,6 +1251,11 @@
       <c r="E8" s="2">
         <v>1</v>
       </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
@@ -1214,13 +1271,18 @@
       <c r="E9" s="2">
         <v>6</v>
       </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -1229,6 +1291,11 @@
       <c r="E10" s="2">
         <v>6</v>
       </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
@@ -1250,22 +1317,22 @@
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
@@ -1280,7 +1347,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
@@ -1337,132 +1404,130 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="E18" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
       <c r="E22" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>107</v>
+        <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>110</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E25" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
@@ -1474,29 +1539,29 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E27" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="E28" s="2">
         <v>6</v>
@@ -1504,74 +1569,74 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>49</v>
+        <v>106</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E29" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E30" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="E31" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="E32" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E33" s="2">
         <v>2</v>
@@ -1579,46 +1644,61 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="E34" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="E35" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="3"/>
       <c r="D36" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E36" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1635,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49D8E50-E16B-43C7-A737-D72E991DFD2E}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1646,66 +1726,66 @@
     <col min="3" max="3" width="39.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7265625" customWidth="1"/>
     <col min="5" max="5" width="11.54296875" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.26953125" customWidth="1"/>
-    <col min="12" max="12" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.26953125" customWidth="1"/>
     <col min="14" max="14" width="12.453125" customWidth="1"/>
     <col min="15" max="15" width="30.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="39"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="str">
@@ -1716,25 +1796,25 @@
         <f>'Product backlog'!B3</f>
         <v>Instalar las herramientas de desarrollo</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="29">
+      <c r="D4" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="28">
         <v>6</v>
       </c>
       <c r="G4" s="2">
         <f>'Product backlog'!E3</f>
         <v>1</v>
       </c>
-      <c r="H4" s="29">
+      <c r="H4" s="28">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="2" t="str">
         <f>'Product backlog'!A4</f>
         <v>HT2</v>
@@ -1743,17 +1823,17 @@
         <f>'Product backlog'!B4</f>
         <v>Establecer el estándar de codificación</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="2">
         <f>'Product backlog'!E4</f>
         <v>1</v>
       </c>
-      <c r="H5" s="29"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="29"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="2" t="str">
         <f>'Product backlog'!A5</f>
         <v>HT3</v>
@@ -1762,24 +1842,24 @@
         <f>'Product backlog'!B5</f>
         <v>Establecer el diseño de base de datos</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="2">
         <f>'Product backlog'!E5</f>
         <v>6</v>
       </c>
-      <c r="H6" s="29"/>
+      <c r="H6" s="28"/>
       <c r="K6" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L6" s="2">
-        <f>SUM(G4:G37)</f>
-        <v>129</v>
+        <f>SUM(G4:G38)</f>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="29"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="2" t="str">
         <f>'Product backlog'!A6</f>
         <v>HT4</v>
@@ -1788,23 +1868,23 @@
         <f>'Product backlog'!B6</f>
         <v>Configurar los servidores y motores de lenguaje</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="2">
         <f>'Product backlog'!E6</f>
         <v>2</v>
       </c>
-      <c r="H7" s="29"/>
+      <c r="H7" s="28"/>
       <c r="K7" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L7" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="29"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="2" t="str">
         <f>'Product backlog'!A7</f>
         <v>HT5</v>
@@ -1813,24 +1893,24 @@
         <f>'Product backlog'!B7</f>
         <v>Configurar repositorio GitHub</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="2">
         <f>'Product backlog'!E7</f>
         <v>1</v>
       </c>
-      <c r="H8" s="29"/>
+      <c r="H8" s="28"/>
       <c r="K8" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L8" s="2">
         <f>L6/L7</f>
-        <v>10.75</v>
+        <v>12.416666666666666</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="29"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="2" t="str">
         <f>'Product backlog'!A8</f>
         <v>HT6</v>
@@ -1839,65 +1919,65 @@
         <f>'Product backlog'!B8</f>
         <v>Implementar la base de datos</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="2">
         <f>'Product backlog'!E8</f>
         <v>1</v>
       </c>
-      <c r="H9" s="29"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="20">
+      <c r="A10" s="19">
         <v>2</v>
       </c>
-      <c r="B10" s="13" t="str">
+      <c r="B10" s="11" t="str">
         <f>'Product backlog'!A9</f>
         <v>HT7</v>
       </c>
-      <c r="C10" s="13" t="str">
+      <c r="C10" s="11" t="str">
         <f>'Product backlog'!B9</f>
         <v>Establecer el diseño de las interfaces</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="30">
+      <c r="D10" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="29">
         <v>45363</v>
       </c>
-      <c r="F10" s="24">
-        <v>6</v>
-      </c>
-      <c r="G10" s="14">
+      <c r="F10" s="23">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2">
         <f>'Product backlog'!E9</f>
         <v>6</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="23">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
-      <c r="B11" s="13" t="str">
+      <c r="A11" s="20"/>
+      <c r="B11" s="11" t="str">
         <f>'Product backlog'!A10</f>
         <v>HT8</v>
       </c>
-      <c r="C11" s="13" t="str">
+      <c r="C11" s="11" t="str">
         <f>'Product backlog'!B10</f>
         <v>Aprendizaje del framework FastAPI y React</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="14">
+      <c r="D11" s="24"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="2">
         <f>'Product backlog'!E10</f>
         <v>6</v>
       </c>
-      <c r="H11" s="25"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="20">
+      <c r="A12" s="19">
         <v>3</v>
       </c>
       <c r="B12" s="3" t="str">
@@ -1908,25 +1988,25 @@
         <f>'Product backlog'!B11</f>
         <v>Visualizar la página principal</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="21">
         <v>45363</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="21">
         <v>45577</v>
       </c>
-      <c r="F12" s="20">
-        <v>6</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="F12" s="19">
+        <v>6</v>
+      </c>
+      <c r="G12" s="2">
         <f>'Product backlog'!E11</f>
         <v>3</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="19">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="21"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="3" t="str">
         <f>'Product backlog'!A12</f>
         <v>HU2</v>
@@ -1935,613 +2015,631 @@
         <f>'Product backlog'!B12</f>
         <v>Gestionar registro y autenticacion de usuarios</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="3">
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="2">
+        <f>'Product backlog'!E12</f>
         <v>9</v>
       </c>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="1:12" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="32">
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="19">
         <v>4</v>
       </c>
-      <c r="B14" s="11" t="str">
+      <c r="B14" s="3" t="str">
         <f>'Product backlog'!A13</f>
-        <v>HU23</v>
-      </c>
-      <c r="C14" s="11" t="str">
+        <v>HU22</v>
+      </c>
+      <c r="C14" s="3" t="str">
         <f>'Product backlog'!B13</f>
         <v>Reestablecer y actualizar contraseña</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="21">
         <v>45577</v>
       </c>
-      <c r="E14" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="32">
-        <v>6</v>
-      </c>
-      <c r="G14" s="11">
+      <c r="E14" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="19">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2">
         <f>'Product backlog'!E13</f>
         <v>4</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="19">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="41"/>
-      <c r="B15" s="11" t="str">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="31"/>
+      <c r="B15" s="3" t="str">
         <f>'Product backlog'!A14</f>
         <v>HU3</v>
       </c>
-      <c r="C15" s="11" t="str">
+      <c r="C15" s="3" t="str">
         <f>'Product backlog'!B14</f>
         <v>Visualizar panel de inicio</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="11">
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="2">
         <f>'Product backlog'!E14</f>
         <v>2</v>
       </c>
-      <c r="H15" s="41"/>
-    </row>
-    <row r="16" spans="1:12" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
-      <c r="B16" s="11" t="str">
+      <c r="H15" s="31"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="20"/>
+      <c r="B16" s="3" t="str">
         <f>'Product backlog'!A15</f>
         <v>HU5</v>
       </c>
-      <c r="C16" s="11" t="str">
+      <c r="C16" s="3" t="str">
         <f>'Product backlog'!B15</f>
         <v>Gestionar membresías</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="11">
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="2">
         <f>'Product backlog'!E15</f>
         <v>8</v>
       </c>
-      <c r="H16" s="33"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="20">
+      <c r="A17" s="33">
         <v>5</v>
       </c>
-      <c r="B17" s="3" t="str">
+      <c r="B17" s="10" t="str">
         <f>'Product backlog'!A16</f>
         <v>HU6</v>
       </c>
-      <c r="C17" s="3" t="str">
+      <c r="C17" s="10" t="str">
         <f>'Product backlog'!B16</f>
         <v>Visualizar membresías disponibles</v>
       </c>
-      <c r="D17" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17" s="20">
-        <v>6</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="D17" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="33">
+        <v>6</v>
+      </c>
+      <c r="G17" s="10">
         <f>'Product backlog'!E16</f>
         <v>2</v>
       </c>
-      <c r="H17" s="20">
-        <v>8</v>
+      <c r="H17" s="33">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="21"/>
-      <c r="B18" s="3" t="str">
+      <c r="A18" s="40"/>
+      <c r="B18" s="10" t="str">
         <f>'Product backlog'!A17</f>
         <v>HU7</v>
       </c>
-      <c r="C18" s="3" t="str">
+      <c r="C18" s="10" t="str">
         <f>'Product backlog'!B17</f>
         <v>Comprar membresía</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="3">
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="10">
         <f>'Product backlog'!E17</f>
         <v>6</v>
       </c>
-      <c r="H18" s="21"/>
+      <c r="H18" s="40"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="20">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3" t="str">
+      <c r="A19" s="40"/>
+      <c r="B19" s="10" t="str">
         <f>'Product backlog'!A18</f>
+        <v>HU8</v>
+      </c>
+      <c r="C19" s="10" t="str">
+        <f>'Product backlog'!B18</f>
+        <v>Visualizar estado de la membresía adquirida</v>
+      </c>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="10">
+        <f>'Product backlog'!E18</f>
+        <v>2</v>
+      </c>
+      <c r="H19" s="40"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="35">
+        <v>6</v>
+      </c>
+      <c r="B20" s="12" t="str">
+        <f>'Product backlog'!A19</f>
+        <v>HT12</v>
+      </c>
+      <c r="C20" s="12" t="str">
+        <f>'Product backlog'!B19</f>
+        <v>Implementación de JWT</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="35">
+        <v>6</v>
+      </c>
+      <c r="G20" s="12">
+        <f>'Product backlog'!E19</f>
+        <v>6</v>
+      </c>
+      <c r="H20" s="35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="35"/>
+      <c r="B21" s="12" t="str">
+        <f>'Product backlog'!A20</f>
+        <v>HU19</v>
+      </c>
+      <c r="C21" s="12" t="str">
+        <f>'Product backlog'!B20</f>
+        <v>Gestionar sueldo Básico</v>
+      </c>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="12">
+        <f>'Product backlog'!E20</f>
+        <v>1</v>
+      </c>
+      <c r="H21" s="35"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="35"/>
+      <c r="B22" s="42" t="str">
+        <f>'Product backlog'!A21</f>
         <v>HU20</v>
       </c>
-      <c r="C19" s="3" t="str">
-        <f>'Product backlog'!B18</f>
-        <v>Visualizar y Modificar sueldo Básico</v>
-      </c>
-      <c r="D19" s="22" t="s">
+      <c r="C22" s="42" t="str">
+        <f>'Product backlog'!B21</f>
+        <v>Gestionar categorías de gastos</v>
+      </c>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="12">
+        <f>'Product backlog'!E21</f>
+        <v>5</v>
+      </c>
+      <c r="H22" s="35"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="44">
+        <v>7</v>
+      </c>
+      <c r="B23" s="13" t="str">
+        <f>'Product backlog'!A22</f>
+        <v>HT13</v>
+      </c>
+      <c r="C23" s="13" t="str">
+        <f>'Product backlog'!B22</f>
+        <v>Redefinición de las tecnologías del front-end</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="45">
+        <v>45839</v>
+      </c>
+      <c r="F23" s="44">
+        <v>6</v>
+      </c>
+      <c r="G23" s="13">
+        <f>'Product backlog'!E22</f>
+        <v>8</v>
+      </c>
+      <c r="H23" s="44">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="44"/>
+      <c r="B24" s="43" t="str">
+        <f>'Product backlog'!A23</f>
+        <v>HU9</v>
+      </c>
+      <c r="C24" s="43" t="str">
+        <f>'Product backlog'!B23</f>
+        <v>Extraer comprobantes electrónicos</v>
+      </c>
+      <c r="D24" s="44"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="13">
+        <f>'Product backlog'!E23</f>
+        <v>10</v>
+      </c>
+      <c r="H24" s="44"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="19">
+        <v>8</v>
+      </c>
+      <c r="B25" s="46" t="str">
+        <f>'Product backlog'!A24</f>
+        <v>HU10</v>
+      </c>
+      <c r="C25" s="46" t="str">
+        <f>'Product backlog'!B24</f>
+        <v>Carga de comprobantes electrónicos</v>
+      </c>
+      <c r="D25" s="21">
+        <v>45839</v>
+      </c>
+      <c r="E25" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" s="20">
-        <v>6</v>
-      </c>
-      <c r="G19" s="3">
-        <f>'Product backlog'!E18</f>
-        <v>1</v>
-      </c>
-      <c r="H19" s="20">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="36"/>
-      <c r="B20" s="3" t="str">
-        <f>'Product backlog'!A19</f>
-        <v>HU21</v>
-      </c>
-      <c r="C20" s="3" t="str">
-        <f>'Product backlog'!B19</f>
-        <v>Gestionar categorías de gastos</v>
-      </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="3">
-        <f>'Product backlog'!E19</f>
-        <v>5</v>
-      </c>
-      <c r="H20" s="36"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="21"/>
-      <c r="B21" s="3" t="str">
-        <f>'Product backlog'!A20</f>
-        <v>HU9</v>
-      </c>
-      <c r="C21" s="3" t="str">
-        <f>'Product backlog'!B20</f>
-        <v>Extraer comprobantes electrónicos</v>
-      </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="3">
-        <f>'Product backlog'!E20</f>
-        <v>5</v>
-      </c>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="20">
-        <v>7</v>
-      </c>
-      <c r="B22" s="3" t="str">
-        <f>'Product backlog'!A21</f>
-        <v>HU10</v>
-      </c>
-      <c r="C22" s="3" t="str">
-        <f>'Product backlog'!B21</f>
-        <v>Carga de comprobantes electrónicos</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="22">
-        <v>45839</v>
-      </c>
-      <c r="F22" s="20">
-        <v>6</v>
-      </c>
-      <c r="G22" s="3">
-        <f>'Product backlog'!E21</f>
+      <c r="F25" s="19">
+        <v>6</v>
+      </c>
+      <c r="G25" s="2">
+        <f>'Product backlog'!E24</f>
         <v>4</v>
       </c>
-      <c r="H22" s="20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="21"/>
-      <c r="B23" s="3" t="str">
-        <f>'Product backlog'!A22</f>
+      <c r="H25" s="19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="31"/>
+      <c r="B26" s="46" t="str">
+        <f>'Product backlog'!A25</f>
         <v>HU11</v>
       </c>
-      <c r="C23" s="3" t="str">
-        <f>'Product backlog'!B22</f>
+      <c r="C26" s="46" t="str">
+        <f>'Product backlog'!B25</f>
         <v>Listar comprobantes cargados</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="3">
-        <f>'Product backlog'!E22</f>
-        <v>3</v>
-      </c>
-      <c r="H23" s="21"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="20">
-        <v>8</v>
-      </c>
-      <c r="B24" s="3" t="str">
-        <f>'Product backlog'!A23</f>
-        <v>HU12</v>
-      </c>
-      <c r="C24" s="3" t="str">
-        <f>'Product backlog'!B23</f>
-        <v>Asignar categoría al comprobante</v>
-      </c>
-      <c r="D24" s="22">
-        <v>45839</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="20">
-        <v>6</v>
-      </c>
-      <c r="G24" s="3">
-        <f>'Product backlog'!E23</f>
-        <v>2</v>
-      </c>
-      <c r="H24" s="20">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="36"/>
-      <c r="B25" s="3" t="str">
-        <f>'Product backlog'!A24</f>
-        <v>HU14</v>
-      </c>
-      <c r="C25" s="3" t="str">
-        <f>'Product backlog'!B24</f>
-        <v>Generar documento deducción de impuestos</v>
-      </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="3">
-        <f>'Product backlog'!E24</f>
-        <v>5</v>
-      </c>
-      <c r="H25" s="36"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="36"/>
-      <c r="B26" s="3" t="str">
-        <f>'Product backlog'!A25</f>
-        <v>HU22</v>
-      </c>
-      <c r="C26" s="3" t="str">
-        <f>'Product backlog'!B25</f>
-        <v>Ver detalles y descargar Documento de Deducción</v>
-      </c>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="3">
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="2">
         <f>'Product backlog'!E25</f>
-        <v>6</v>
-      </c>
-      <c r="H26" s="36"/>
+        <v>4</v>
+      </c>
+      <c r="H26" s="31"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="21"/>
-      <c r="B27" s="3" t="str">
+      <c r="A27" s="31"/>
+      <c r="B27" s="46" t="str">
         <f>'Product backlog'!A26</f>
-        <v>HU18</v>
-      </c>
-      <c r="C27" s="3" t="str">
+        <v>HU13</v>
+      </c>
+      <c r="C27" s="46" t="str">
         <f>'Product backlog'!B26</f>
-        <v>Visualizar y modificar datos del administrador</v>
-      </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="3">
+        <v>Visualizar comprobante específico</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="2">
         <f>'Product backlog'!E26</f>
         <v>2</v>
       </c>
-      <c r="H27" s="21"/>
+      <c r="H27" s="31"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="20">
-        <v>9</v>
-      </c>
+      <c r="A28" s="20"/>
       <c r="B28" s="3" t="str">
         <f>'Product backlog'!A27</f>
-        <v>HT9</v>
+        <v>HU12</v>
       </c>
       <c r="C28" s="3" t="str">
         <f>'Product backlog'!B27</f>
-        <v>Implementar el modelo de machine learning</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" s="20">
-        <v>6</v>
-      </c>
-      <c r="G28" s="3">
+        <v>Asignar categoría al comprobante</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="2">
         <f>'Product backlog'!E27</f>
-        <v>6</v>
-      </c>
-      <c r="H28" s="20">
-        <v>12</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H28" s="20"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="21"/>
+      <c r="A29" s="28">
+        <v>9</v>
+      </c>
       <c r="B29" s="3" t="str">
         <f>'Product backlog'!A28</f>
-        <v>HU17</v>
+        <v>HU14</v>
       </c>
       <c r="C29" s="3" t="str">
         <f>'Product backlog'!B28</f>
-        <v>Visualizar predicción de gastos</v>
-      </c>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="3">
+        <v>Generar documento deducción de impuestos</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="28">
+        <v>6</v>
+      </c>
+      <c r="G29" s="2">
         <f>'Product backlog'!E28</f>
         <v>6</v>
       </c>
-      <c r="H29" s="21"/>
+      <c r="H29" s="28">
+        <v>10</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="20">
-        <v>10</v>
-      </c>
+      <c r="A30" s="28"/>
       <c r="B30" s="3" t="str">
         <f>'Product backlog'!A29</f>
-        <v>HU13</v>
+        <v>HU21</v>
       </c>
       <c r="C30" s="3" t="str">
         <f>'Product backlog'!B29</f>
-        <v>Visualizar comprobante específico</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" s="20">
-        <v>5</v>
-      </c>
-      <c r="G30" s="3">
+        <v>Ver detalles y descargar Documento de Deducción</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="2">
         <f>'Product backlog'!E29</f>
-        <v>2</v>
-      </c>
-      <c r="H30" s="20">
-        <v>7</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="H30" s="28"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="36"/>
+      <c r="A31" s="28">
+        <v>10</v>
+      </c>
       <c r="B31" s="3" t="str">
         <f>'Product backlog'!A30</f>
-        <v>HU8</v>
+        <v>HT9</v>
       </c>
       <c r="C31" s="3" t="str">
         <f>'Product backlog'!B30</f>
-        <v>Visualizar estado de la membresía adquirida</v>
-      </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="3">
+        <v>Implementar el modelo de machine learning</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="28">
+        <v>5</v>
+      </c>
+      <c r="G31" s="2">
         <f>'Product backlog'!E30</f>
-        <v>2</v>
-      </c>
-      <c r="H31" s="36"/>
+        <v>7</v>
+      </c>
+      <c r="H31" s="28">
+        <v>14</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="21"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="3" t="str">
         <f>'Product backlog'!A31</f>
-        <v>HU4</v>
+        <v>HU16</v>
       </c>
       <c r="C32" s="3" t="str">
         <f>'Product backlog'!B31</f>
-        <v>Visualizar y modificar datos del usuario</v>
-      </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="3">
+        <v>Visualizar predicción de gastos</v>
+      </c>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="2">
         <f>'Product backlog'!E31</f>
-        <v>3</v>
-      </c>
-      <c r="H32" s="21"/>
+        <v>7</v>
+      </c>
+      <c r="H32" s="28"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="20">
+      <c r="A33" s="28">
         <v>11</v>
       </c>
       <c r="B33" s="3" t="str">
         <f>'Product backlog'!A32</f>
-        <v>HU15</v>
+        <v>HU4</v>
       </c>
       <c r="C33" s="3" t="str">
         <f>'Product backlog'!B32</f>
-        <v>Visualizar historial de deducciones</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" s="22">
+        <v>Visualizar y modificar datos del usuario</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="47">
         <v>45749</v>
       </c>
-      <c r="F33" s="20">
-        <v>6</v>
-      </c>
-      <c r="G33" s="3">
+      <c r="F33" s="28">
+        <v>6</v>
+      </c>
+      <c r="G33" s="2">
         <f>'Product backlog'!E32</f>
-        <v>2</v>
-      </c>
-      <c r="H33" s="20">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="H33" s="28">
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="36"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="3" t="str">
         <f>'Product backlog'!A33</f>
-        <v>HU19</v>
+        <v>HU15</v>
       </c>
       <c r="C34" s="3" t="str">
         <f>'Product backlog'!B33</f>
-        <v>Listar clientes registrados</v>
-      </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="3">
+        <v>Visualizar historial de deducciones</v>
+      </c>
+      <c r="D34" s="28"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="2">
         <f>'Product backlog'!E33</f>
         <v>2</v>
       </c>
-      <c r="H34" s="36"/>
+      <c r="H34" s="28"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="21"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="3" t="str">
         <f>'Product backlog'!A34</f>
-        <v>HU16</v>
+        <v>HU18</v>
       </c>
       <c r="C35" s="3" t="str">
         <f>'Product backlog'!B34</f>
-        <v>Darse de baja del sistema</v>
-      </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="3">
+        <v>Listar clientes registrados</v>
+      </c>
+      <c r="D35" s="28"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="2">
         <f>'Product backlog'!E34</f>
-        <v>3</v>
-      </c>
-      <c r="H35" s="21"/>
+        <v>2</v>
+      </c>
+      <c r="H35" s="28"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="20">
-        <v>12</v>
-      </c>
-      <c r="B36" s="5" t="str">
+      <c r="A36" s="28"/>
+      <c r="B36" s="3" t="str">
         <f>'Product backlog'!A35</f>
-        <v>HT10</v>
+        <v>HU17</v>
       </c>
       <c r="C36" s="3" t="str">
         <f>'Product backlog'!B35</f>
+        <v>Visualizar y modificar datos del administrador</v>
+      </c>
+      <c r="D36" s="28"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="2">
+        <f>'Product backlog'!E35</f>
+        <v>4</v>
+      </c>
+      <c r="H36" s="28"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="19">
+        <v>12</v>
+      </c>
+      <c r="B37" s="4" t="str">
+        <f>'Product backlog'!A36</f>
+        <v>HT10</v>
+      </c>
+      <c r="C37" s="3" t="str">
+        <f>'Product backlog'!B36</f>
         <v>Refactorización del código</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D37" s="21">
         <v>45748</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E37" s="21">
         <v>45901</v>
       </c>
-      <c r="F36" s="20">
+      <c r="F37" s="19">
         <v>5</v>
       </c>
-      <c r="G36" s="4">
-        <f>'Product backlog'!E35</f>
-        <v>6</v>
-      </c>
-      <c r="H36" s="20">
+      <c r="G37" s="2">
+        <f>'Product backlog'!E36</f>
+        <v>6</v>
+      </c>
+      <c r="H37" s="19">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="21"/>
-      <c r="B37" s="5" t="str">
-        <f>'Product backlog'!A36</f>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="20"/>
+      <c r="B38" s="4" t="str">
+        <f>'Product backlog'!A37</f>
         <v>HT11</v>
       </c>
-      <c r="C37" s="5" t="str">
-        <f>'Product backlog'!B36</f>
+      <c r="C38" s="4" t="str">
+        <f>'Product backlog'!B37</f>
         <v>Despliegue y puesta a punto</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="4">
-        <f>'Product backlog'!E36</f>
-        <v>6</v>
-      </c>
-      <c r="H37" s="21"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="2">
+        <f>'Product backlog'!E37</f>
+        <v>6</v>
+      </c>
+      <c r="H38" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D25:D28"/>
+    <mergeCell ref="E25:E28"/>
+    <mergeCell ref="F25:F28"/>
+    <mergeCell ref="H25:H28"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H33:H36"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="F33:F36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="H37:H38"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="H30:H32"/>
-    <mergeCell ref="H33:H35"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="F14:F16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="D12:D13"/>
@@ -2556,6 +2654,8 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
actualizacion esquema db e historias
</commit_message>
<xml_diff>
--- a/documentacion/scrum/Product backlog.xlsx
+++ b/documentacion/scrum/Product backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyecto\documentacion\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A785EE-2B12-4A12-99EE-761ED156BA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E5CE2C-1AED-455C-8772-C9AEDC96E92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{62494E98-7055-48D3-B966-884A22B78DF5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{62494E98-7055-48D3-B966-884A22B78DF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="122">
   <si>
     <t>Product backlog</t>
   </si>
@@ -192,9 +192,6 @@
     <t>HU14</t>
   </si>
   <si>
-    <t>Generar documento deducción de impuestos</t>
-  </si>
-  <si>
     <t>HU15</t>
   </si>
   <si>
@@ -204,12 +201,6 @@
     <t>HU17</t>
   </si>
   <si>
-    <t>Visualizar historial de deducciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baja </t>
-  </si>
-  <si>
     <t>HU18</t>
   </si>
   <si>
@@ -354,9 +345,6 @@
     <t>Requisitos</t>
   </si>
   <si>
-    <t>Ver detalles y descargar Documento de Deducción</t>
-  </si>
-  <si>
     <t>Reestablecer y actualizar contraseña</t>
   </si>
   <si>
@@ -366,9 +354,6 @@
     <t>HT12</t>
   </si>
   <si>
-    <t>Gestionar sueldo Básico</t>
-  </si>
-  <si>
     <t>HT13</t>
   </si>
   <si>
@@ -394,13 +379,40 @@
   </si>
   <si>
     <t>Diseñar diagrama de actividades</t>
+  </si>
+  <si>
+    <t>Gestionar fracción básica desgravada</t>
+  </si>
+  <si>
+    <t>Generar y Descargar Anexo de Gastos Personales</t>
+  </si>
+  <si>
+    <t>RF16, RF25</t>
+  </si>
+  <si>
+    <t>Gestionar Periodos Fiscales</t>
+  </si>
+  <si>
+    <t>RF26</t>
+  </si>
+  <si>
+    <t>RF21</t>
+  </si>
+  <si>
+    <t>Gestionar Configuración del Sistema</t>
+  </si>
+  <si>
+    <t>20/01/2024</t>
+  </si>
+  <si>
+    <t>Añadir historia de gestion de la configuracion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,6 +433,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -462,7 +480,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -612,19 +630,61 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -636,63 +696,18 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3399"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1023,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A306DB25-FA75-4E4E-8913-B4C3461E94DB}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1034,7 +1049,7 @@
     <col min="4" max="4" width="8.54296875" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.1796875" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.453125" customWidth="1"/>
     <col min="11" max="11" width="43.453125" customWidth="1"/>
   </cols>
@@ -1056,17 +1071,17 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
@@ -1088,16 +1103,16 @@
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>2</v>
@@ -1118,19 +1133,19 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H4" s="2">
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1148,19 +1163,19 @@
         <v>6</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H5" s="2">
         <v>2</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1184,13 +1199,13 @@
         <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1214,13 +1229,13 @@
         <v>4</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -1237,11 +1252,21 @@
       <c r="E8" s="2">
         <v>1</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
@@ -1268,7 +1293,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -1303,7 +1328,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
@@ -1315,10 +1340,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
@@ -1333,7 +1358,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
@@ -1405,10 +1430,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
@@ -1420,70 +1445,70 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="E21" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="2">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>117</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
@@ -1495,10 +1520,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
@@ -1510,29 +1535,29 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="E26" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E27" s="2">
         <v>2</v>
@@ -1540,47 +1565,53 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C28" s="2"/>
+        <v>116</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>118</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>115</v>
+      </c>
       <c r="D30" s="2" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E30" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1600,10 +1631,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
@@ -1615,44 +1646,44 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E33" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="E34" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E35" s="2">
         <v>2</v>
@@ -1660,10 +1691,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
@@ -1678,7 +1709,7 @@
         <v>23</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="2" t="s">
@@ -1690,10 +1721,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
@@ -1718,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49D8E50-E16B-43C7-A737-D72E991DFD2E}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1736,57 +1767,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33"/>
+      <c r="A1" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="39" t="s">
+      <c r="F3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="19">
+      <c r="A4" s="30">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="str">
@@ -1797,25 +1828,25 @@
         <f>'Product backlog'!B3</f>
         <v>Instalar las herramientas de desarrollo</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="19">
+      <c r="D4" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="30">
         <v>6</v>
       </c>
       <c r="G4" s="2">
         <f>'Product backlog'!E3</f>
         <v>1</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="30">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="19"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="2" t="str">
         <f>'Product backlog'!A4</f>
         <v>HT2</v>
@@ -1824,17 +1855,17 @@
         <f>'Product backlog'!B4</f>
         <v>Establecer el estándar de codificación</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="2">
         <f>'Product backlog'!E4</f>
         <v>1</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="2" t="str">
         <f>'Product backlog'!A5</f>
         <v>HT3</v>
@@ -1843,24 +1874,24 @@
         <f>'Product backlog'!B5</f>
         <v>Establecer el diseño de base de datos</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
       <c r="G6" s="2">
         <f>'Product backlog'!E5</f>
         <v>6</v>
       </c>
-      <c r="H6" s="19"/>
+      <c r="H6" s="30"/>
       <c r="K6" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L6" s="2">
         <f>SUM(G4:G39)</f>
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="2" t="str">
         <f>'Product backlog'!A6</f>
         <v>HT4</v>
@@ -1869,23 +1900,23 @@
         <f>'Product backlog'!B6</f>
         <v>Configurar los servidores y motores de lenguaje</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="2">
         <f>'Product backlog'!E6</f>
         <v>2</v>
       </c>
-      <c r="H7" s="19"/>
+      <c r="H7" s="30"/>
       <c r="K7" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L7" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="19"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="2" t="str">
         <f>'Product backlog'!A7</f>
         <v>HT5</v>
@@ -1894,24 +1925,24 @@
         <f>'Product backlog'!B7</f>
         <v>Configurar repositorio GitHub</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="2">
         <f>'Product backlog'!E7</f>
         <v>1</v>
       </c>
-      <c r="H8" s="19"/>
+      <c r="H8" s="30"/>
       <c r="K8" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L8" s="2">
         <f>L6/L7</f>
-        <v>12.833333333333334</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="2" t="str">
         <f>'Product backlog'!A8</f>
         <v>HT6</v>
@@ -1920,17 +1951,17 @@
         <f>'Product backlog'!B8</f>
         <v>Implementar la base de datos</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
       <c r="G9" s="2">
         <f>'Product backlog'!E8</f>
         <v>1</v>
       </c>
-      <c r="H9" s="19"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="27">
+      <c r="A10" s="19">
         <v>2</v>
       </c>
       <c r="B10" s="10" t="str">
@@ -1941,25 +1972,25 @@
         <f>'Product backlog'!B9</f>
         <v>Establecer el diseño de las interfaces</v>
       </c>
-      <c r="D10" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="42">
+      <c r="D10" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="31">
         <v>45363</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="25">
         <v>6</v>
       </c>
       <c r="G10" s="2">
         <f>'Product backlog'!E9</f>
         <v>6</v>
       </c>
-      <c r="H10" s="37">
+      <c r="H10" s="25">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="10" t="str">
         <f>'Product backlog'!A10</f>
         <v>HT8</v>
@@ -1968,17 +1999,17 @@
         <f>'Product backlog'!B10</f>
         <v>Aprendizaje del framework FastAPI y React</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="38"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="26"/>
       <c r="G11" s="2">
         <f>'Product backlog'!E10</f>
         <v>6</v>
       </c>
-      <c r="H11" s="38"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="27">
+      <c r="A12" s="19">
         <v>3</v>
       </c>
       <c r="B12" s="3" t="str">
@@ -1989,25 +2020,25 @@
         <f>'Product backlog'!B11</f>
         <v>Visualizar la página principal</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="22">
         <v>45363</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="22">
         <v>45577</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="19">
         <v>6</v>
       </c>
       <c r="G12" s="2">
         <f>'Product backlog'!E11</f>
         <v>3</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="19">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="3" t="str">
         <f>'Product backlog'!A12</f>
         <v>HU2</v>
@@ -2016,17 +2047,17 @@
         <f>'Product backlog'!B12</f>
         <v>Gestionar registro y autenticacion de usuarios</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="28"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="2">
         <f>'Product backlog'!E12</f>
         <v>9</v>
       </c>
-      <c r="H13" s="28"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="27">
+      <c r="A14" s="19">
         <v>4</v>
       </c>
       <c r="B14" s="3" t="str">
@@ -2037,25 +2068,25 @@
         <f>'Product backlog'!B13</f>
         <v>Reestablecer y actualizar contraseña</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="22">
         <v>45577</v>
       </c>
-      <c r="E14" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="27">
+      <c r="E14" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="19">
         <v>6</v>
       </c>
       <c r="G14" s="2">
         <f>'Product backlog'!E13</f>
         <v>4</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="19">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="34"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="3" t="str">
         <f>'Product backlog'!A14</f>
         <v>HU3</v>
@@ -2064,17 +2095,17 @@
         <f>'Product backlog'!B14</f>
         <v>Visualizar panel de inicio</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="34"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="2">
         <f>'Product backlog'!E14</f>
         <v>2</v>
       </c>
-      <c r="H15" s="34"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="3" t="str">
         <f>'Product backlog'!A15</f>
         <v>HU5</v>
@@ -2083,17 +2114,17 @@
         <f>'Product backlog'!B15</f>
         <v>Gestionar membresías</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="28"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="2">
         <f>'Product backlog'!E15</f>
         <v>8</v>
       </c>
-      <c r="H16" s="28"/>
+      <c r="H16" s="21"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="19">
+      <c r="A17" s="30">
         <v>5</v>
       </c>
       <c r="B17" s="3" t="str">
@@ -2104,25 +2135,25 @@
         <f>'Product backlog'!B16</f>
         <v>Visualizar membresías disponibles</v>
       </c>
-      <c r="D17" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="19">
+      <c r="D17" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="30">
         <v>6</v>
       </c>
       <c r="G17" s="3">
         <f>'Product backlog'!E16</f>
         <v>2</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="30">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="19"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="3" t="str">
         <f>'Product backlog'!A17</f>
         <v>HU7</v>
@@ -2131,17 +2162,17 @@
         <f>'Product backlog'!B17</f>
         <v>Comprar membresía</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="19"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="30"/>
       <c r="G18" s="3">
         <f>'Product backlog'!E17</f>
         <v>6</v>
       </c>
-      <c r="H18" s="19"/>
+      <c r="H18" s="30"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="19"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="3" t="str">
         <f>'Product backlog'!A18</f>
         <v>HU8</v>
@@ -2150,14 +2181,14 @@
         <f>'Product backlog'!B18</f>
         <v>Visualizar estado de la membresía adquirida</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="19"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="3">
         <f>'Product backlog'!E18</f>
         <v>2</v>
       </c>
-      <c r="H19" s="19"/>
+      <c r="H19" s="30"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="19">
@@ -2171,11 +2202,11 @@
         <f>'Product backlog'!B19</f>
         <v>Implementación de JWT</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>79</v>
+      <c r="D20" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>76</v>
       </c>
       <c r="F20" s="19">
         <v>6</v>
@@ -2185,247 +2216,247 @@
         <v>6</v>
       </c>
       <c r="H20" s="19">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="19"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="3" t="str">
         <f>'Product backlog'!A20</f>
-        <v>HU19</v>
+        <v>HU20</v>
       </c>
       <c r="C21" s="3" t="str">
         <f>'Product backlog'!B20</f>
-        <v>Gestionar sueldo Básico</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="19"/>
+        <v>Gestionar categorías de gastos</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="21"/>
       <c r="G21" s="3">
         <f>'Product backlog'!E20</f>
-        <v>2</v>
-      </c>
-      <c r="H21" s="19"/>
+        <v>5</v>
+      </c>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="19"/>
+      <c r="A22" s="30">
+        <v>7</v>
+      </c>
       <c r="B22" s="3" t="str">
         <f>'Product backlog'!A21</f>
-        <v>HU20</v>
+        <v>HT13</v>
       </c>
       <c r="C22" s="3" t="str">
         <f>'Product backlog'!B21</f>
-        <v>Gestionar categorías de gastos</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="19"/>
+        <v>Redefinición de las tecnologías del front-end</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="36">
+        <v>45839</v>
+      </c>
+      <c r="F22" s="30">
+        <v>6</v>
+      </c>
       <c r="G22" s="3">
         <f>'Product backlog'!E21</f>
-        <v>5</v>
-      </c>
-      <c r="H22" s="19"/>
+        <v>8</v>
+      </c>
+      <c r="H22" s="30">
+        <v>18</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="19">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3" t="str">
+      <c r="A23" s="30"/>
+      <c r="B23" s="4" t="str">
         <f>'Product backlog'!A22</f>
-        <v>HT13</v>
-      </c>
-      <c r="C23" s="3" t="str">
+        <v>HU9</v>
+      </c>
+      <c r="C23" s="4" t="str">
         <f>'Product backlog'!B22</f>
-        <v>Redefinición de las tecnologías del front-end</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" s="20">
-        <v>45839</v>
-      </c>
-      <c r="F23" s="19">
-        <v>6</v>
-      </c>
+        <v>Extraer comprobantes electrónicos</v>
+      </c>
+      <c r="D23" s="30"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="30"/>
       <c r="G23" s="3">
         <f>'Product backlog'!E22</f>
+        <v>10</v>
+      </c>
+      <c r="H23" s="30"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="19">
         <v>8</v>
       </c>
-      <c r="H23" s="19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="19"/>
-      <c r="B24" s="4" t="str">
+      <c r="B24" s="3" t="str">
         <f>'Product backlog'!A23</f>
-        <v>HU9</v>
-      </c>
-      <c r="C24" s="4" t="str">
+        <v>HT14</v>
+      </c>
+      <c r="C24" s="3" t="str">
         <f>'Product backlog'!B23</f>
-        <v>Extraer comprobantes electrónicos</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="3">
+        <v>Diseñar diagrama de actividades</v>
+      </c>
+      <c r="D24" s="22">
+        <v>45839</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="19">
+        <v>6</v>
+      </c>
+      <c r="G24" s="2">
         <f>'Product backlog'!E23</f>
-        <v>10</v>
-      </c>
-      <c r="H24" s="19"/>
+        <v>4</v>
+      </c>
+      <c r="H24" s="19">
+        <v>16</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="24">
-        <v>8</v>
-      </c>
-      <c r="B25" s="13" t="str">
+      <c r="A25" s="20"/>
+      <c r="B25" s="3" t="str">
         <f>'Product backlog'!A24</f>
-        <v>HT14</v>
-      </c>
-      <c r="C25" s="13" t="str">
+        <v>HU10</v>
+      </c>
+      <c r="C25" s="3" t="str">
         <f>'Product backlog'!B24</f>
-        <v>Diseñar diagrama de actividades</v>
-      </c>
-      <c r="D25" s="21">
-        <v>45839</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" s="24">
-        <v>6</v>
-      </c>
-      <c r="G25" s="14">
+        <v>Carga de comprobantes electrónicos</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="2">
         <f>'Product backlog'!E24</f>
         <v>4</v>
       </c>
-      <c r="H25" s="24">
-        <v>16</v>
-      </c>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="25"/>
-      <c r="B26" s="13" t="str">
+      <c r="A26" s="20"/>
+      <c r="B26" s="3" t="str">
         <f>'Product backlog'!A25</f>
-        <v>HU10</v>
-      </c>
-      <c r="C26" s="13" t="str">
+        <v>HU11</v>
+      </c>
+      <c r="C26" s="3" t="str">
         <f>'Product backlog'!B25</f>
-        <v>Carga de comprobantes electrónicos</v>
-      </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="14">
+        <v>Listar comprobantes cargados</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="2">
         <f>'Product backlog'!E25</f>
         <v>4</v>
       </c>
-      <c r="H26" s="25"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="25"/>
-      <c r="B27" s="13" t="str">
+      <c r="A27" s="20"/>
+      <c r="B27" s="3" t="str">
         <f>'Product backlog'!A26</f>
-        <v>HU11</v>
-      </c>
-      <c r="C27" s="13" t="str">
+        <v>HU13</v>
+      </c>
+      <c r="C27" s="3" t="str">
         <f>'Product backlog'!B26</f>
-        <v>Listar comprobantes cargados</v>
-      </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="14">
+        <v>Visualizar detalles comprobante específico</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="2">
         <f>'Product backlog'!E26</f>
-        <v>4</v>
-      </c>
-      <c r="H27" s="25"/>
+        <v>2</v>
+      </c>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="25"/>
-      <c r="B28" s="13" t="str">
+      <c r="A28" s="21"/>
+      <c r="B28" s="3" t="str">
         <f>'Product backlog'!A27</f>
-        <v>HU13</v>
-      </c>
-      <c r="C28" s="13" t="str">
+        <v>HU12</v>
+      </c>
+      <c r="C28" s="3" t="str">
         <f>'Product backlog'!B27</f>
-        <v>Visualizar detalles comprobante específico</v>
-      </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="14">
+        <v>Asignar categoría a los detalles del comprobante</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="2">
         <f>'Product backlog'!E27</f>
         <v>2</v>
       </c>
-      <c r="H28" s="25"/>
+      <c r="H28" s="21"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="26"/>
+      <c r="A29" s="38">
+        <v>9</v>
+      </c>
       <c r="B29" s="13" t="str">
+        <f>'Product backlog'!A29</f>
+        <v>HU19</v>
+      </c>
+      <c r="C29" s="13" t="str">
+        <f>'Product backlog'!B29</f>
+        <v>Gestionar fracción básica desgravada</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="38">
+        <v>6</v>
+      </c>
+      <c r="G29" s="14">
+        <f>'Product backlog'!E29</f>
+        <v>3</v>
+      </c>
+      <c r="H29" s="38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="39"/>
+      <c r="B30" s="13" t="str">
+        <f>'Product backlog'!A30</f>
+        <v>HU14</v>
+      </c>
+      <c r="C30" s="13" t="str">
+        <f>'Product backlog'!B30</f>
+        <v>Generar y Descargar Anexo de Gastos Personales</v>
+      </c>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="14">
+        <f>'Product backlog'!E30</f>
+        <v>8</v>
+      </c>
+      <c r="H30" s="39"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="40"/>
+      <c r="B31" s="13" t="str">
         <f>'Product backlog'!A28</f>
-        <v>HU12</v>
-      </c>
-      <c r="C29" s="13" t="str">
+        <v>HU21</v>
+      </c>
+      <c r="C31" s="13" t="str">
         <f>'Product backlog'!B28</f>
-        <v>Asignar categoría a los detalles del comprobante</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="14">
+        <v>Gestionar Periodos Fiscales</v>
+      </c>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="14">
         <f>'Product backlog'!E28</f>
-        <v>2</v>
-      </c>
-      <c r="H29" s="26"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="19">
-        <v>9</v>
-      </c>
-      <c r="B30" s="3" t="str">
-        <f>'Product backlog'!A29</f>
-        <v>HU14</v>
-      </c>
-      <c r="C30" s="3" t="str">
-        <f>'Product backlog'!B29</f>
-        <v>Generar documento deducción de impuestos</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F30" s="19">
-        <v>6</v>
-      </c>
-      <c r="G30" s="2">
-        <f>'Product backlog'!E29</f>
-        <v>6</v>
-      </c>
-      <c r="H30" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="19"/>
-      <c r="B31" s="3" t="str">
-        <f>'Product backlog'!A30</f>
-        <v>HU21</v>
-      </c>
-      <c r="C31" s="3" t="str">
-        <f>'Product backlog'!B30</f>
-        <v>Ver detalles y descargar Documento de Deducción</v>
-      </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="2">
-        <f>'Product backlog'!E30</f>
         <v>4</v>
       </c>
-      <c r="H31" s="19"/>
+      <c r="H31" s="40"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="19">
@@ -2440,10 +2471,10 @@
         <v>Implementar el modelo de machine learning</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F32" s="19">
         <v>5</v>
@@ -2453,11 +2484,11 @@
         <v>7</v>
       </c>
       <c r="H32" s="19">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="19"/>
+      <c r="A33" s="20"/>
       <c r="B33" s="3" t="str">
         <f>'Product backlog'!A32</f>
         <v>HU16</v>
@@ -2466,65 +2497,65 @@
         <f>'Product backlog'!B32</f>
         <v>Visualizar predicción de gastos</v>
       </c>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="2">
         <f>'Product backlog'!E32</f>
         <v>7</v>
       </c>
-      <c r="H33" s="19"/>
+      <c r="H33" s="20"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="19">
-        <v>11</v>
-      </c>
+      <c r="A34" s="21"/>
       <c r="B34" s="3" t="str">
         <f>'Product backlog'!A33</f>
-        <v>HU4</v>
+        <v>HU15</v>
       </c>
       <c r="C34" s="3" t="str">
         <f>'Product backlog'!B33</f>
-        <v>Visualizar y modificar datos del usuario</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E34" s="20">
-        <v>45749</v>
-      </c>
-      <c r="F34" s="19">
-        <v>6</v>
-      </c>
+        <v>Gestionar Configuración del Sistema</v>
+      </c>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="2">
         <f>'Product backlog'!E33</f>
-        <v>3</v>
-      </c>
-      <c r="H34" s="19">
+        <v>4</v>
+      </c>
+      <c r="H34" s="21"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="19">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="19"/>
       <c r="B35" s="3" t="str">
         <f>'Product backlog'!A34</f>
-        <v>HU15</v>
+        <v>HU4</v>
       </c>
       <c r="C35" s="3" t="str">
         <f>'Product backlog'!B34</f>
-        <v>Visualizar historial de deducciones</v>
-      </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="19"/>
+        <v>Visualizar y modificar datos del usuario</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="22">
+        <v>45749</v>
+      </c>
+      <c r="F35" s="19">
+        <v>6</v>
+      </c>
       <c r="G35" s="2">
         <f>'Product backlog'!E34</f>
-        <v>2</v>
-      </c>
-      <c r="H35" s="19"/>
+        <v>3</v>
+      </c>
+      <c r="H35" s="19">
+        <v>9</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="19"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="3" t="str">
         <f>'Product backlog'!A35</f>
         <v>HU18</v>
@@ -2533,17 +2564,17 @@
         <f>'Product backlog'!B35</f>
         <v>Listar clientes registrados</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="20"/>
       <c r="G36" s="2">
         <f>'Product backlog'!E35</f>
         <v>2</v>
       </c>
-      <c r="H36" s="19"/>
+      <c r="H36" s="20"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="19"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="3" t="str">
         <f>'Product backlog'!A36</f>
         <v>HU17</v>
@@ -2552,17 +2583,17 @@
         <f>'Product backlog'!B36</f>
         <v>Visualizar y modificar datos del administrador</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="19"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="2">
         <f>'Product backlog'!E36</f>
         <v>4</v>
       </c>
-      <c r="H37" s="19"/>
+      <c r="H37" s="21"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="27">
+      <c r="A38" s="19">
         <v>12</v>
       </c>
       <c r="B38" s="4" t="str">
@@ -2573,25 +2604,25 @@
         <f>'Product backlog'!B37</f>
         <v>Refactorización del código</v>
       </c>
-      <c r="D38" s="29">
+      <c r="D38" s="22">
         <v>45748</v>
       </c>
-      <c r="E38" s="29">
+      <c r="E38" s="22">
         <v>45901</v>
       </c>
-      <c r="F38" s="27">
+      <c r="F38" s="19">
         <v>5</v>
       </c>
       <c r="G38" s="2">
         <f>'Product backlog'!E37</f>
         <v>6</v>
       </c>
-      <c r="H38" s="27">
+      <c r="H38" s="19">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="28"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="4" t="str">
         <f>'Product backlog'!A38</f>
         <v>HT11</v>
@@ -2600,36 +2631,47 @@
         <f>'Product backlog'!B38</f>
         <v>Despliegue y puesta a punto</v>
       </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="28"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="21"/>
       <c r="G39" s="2">
         <f>'Product backlog'!E38</f>
         <v>6</v>
       </c>
-      <c r="H39" s="28"/>
+      <c r="H39" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="H25:H29"/>
-    <mergeCell ref="F25:F29"/>
-    <mergeCell ref="E25:E29"/>
-    <mergeCell ref="D25:D29"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="H4:H9"/>
-    <mergeCell ref="F4:F9"/>
-    <mergeCell ref="D4:D9"/>
-    <mergeCell ref="E4:E9"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="H38:H39"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A17:A19"/>
@@ -2646,36 +2688,25 @@
     <mergeCell ref="F14:F16"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="H4:H9"/>
+    <mergeCell ref="F4:F9"/>
+    <mergeCell ref="D4:D9"/>
+    <mergeCell ref="E4:E9"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H24:H28"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="A24:A28"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correccion final historias y requisitos
</commit_message>
<xml_diff>
--- a/documentacion/scrum/Product backlog.xlsx
+++ b/documentacion/scrum/Product backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyecto\documentacion\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C9982B-609A-4921-B284-DABC5FAF36E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63EF451-73AC-444B-8607-600152528ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{62494E98-7055-48D3-B966-884A22B78DF5}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="158">
   <si>
     <t>Product backlog</t>
   </si>
@@ -408,7 +408,112 @@
     <t>Configuración del Sistema - Intentos Login</t>
   </si>
   <si>
-    <t>Configuración y Modificación del Sistema - Tiempo sesion y Correo</t>
+    <t>Correccion final</t>
+  </si>
+  <si>
+    <t>RF01</t>
+  </si>
+  <si>
+    <t>RF02, RF03</t>
+  </si>
+  <si>
+    <t>RF24</t>
+  </si>
+  <si>
+    <t>RF04</t>
+  </si>
+  <si>
+    <t>RF05, RF06, RF07</t>
+  </si>
+  <si>
+    <t>RF08</t>
+  </si>
+  <si>
+    <t>RF09</t>
+  </si>
+  <si>
+    <t>RF10</t>
+  </si>
+  <si>
+    <t>RF12</t>
+  </si>
+  <si>
+    <t>RF11</t>
+  </si>
+  <si>
+    <t>RF13</t>
+  </si>
+  <si>
+    <t>RF14</t>
+  </si>
+  <si>
+    <t>RF15</t>
+  </si>
+  <si>
+    <t>RF17</t>
+  </si>
+  <si>
+    <t>RF18</t>
+  </si>
+  <si>
+    <t>RF19</t>
+  </si>
+  <si>
+    <t>RF20</t>
+  </si>
+  <si>
+    <t>RF22, RF23</t>
+  </si>
+  <si>
+    <t>HU23</t>
+  </si>
+  <si>
+    <t>RF28, RF29</t>
+  </si>
+  <si>
+    <t>Configuración del sistema - Tiempo sesion y Credenciales Correo</t>
+  </si>
+  <si>
+    <t>RNF1</t>
+  </si>
+  <si>
+    <t>RNF3</t>
+  </si>
+  <si>
+    <t>RNF2</t>
+  </si>
+  <si>
+    <t>RNF4</t>
+  </si>
+  <si>
+    <t>RNF5</t>
+  </si>
+  <si>
+    <t>RNF8</t>
+  </si>
+  <si>
+    <t>RNF7</t>
+  </si>
+  <si>
+    <t>RNF6</t>
+  </si>
+  <si>
+    <t>RNF9</t>
+  </si>
+  <si>
+    <t>RNF10</t>
+  </si>
+  <si>
+    <t>RNF11</t>
+  </si>
+  <si>
+    <t>RNF13</t>
+  </si>
+  <si>
+    <t>RNF12</t>
+  </si>
+  <si>
+    <t>RNF14</t>
   </si>
 </sst>
 </file>
@@ -483,7 +588,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -617,98 +722,105 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1050,14 +1162,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A306DB25-FA75-4E4E-8913-B4C3461E94DB}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="42.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="45.54296875" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" customWidth="1"/>
     <col min="4" max="4" width="8.54296875" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.1796875" customWidth="1"/>
@@ -1067,13 +1179,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -1092,22 +1204,24 @@
         <v>66</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+    </row>
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="47" t="s">
+        <v>144</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1130,14 +1244,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="47" t="s">
+        <v>146</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1160,14 +1276,16 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="47" t="s">
+        <v>145</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1190,14 +1308,16 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="47" t="s">
+        <v>147</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1220,14 +1340,16 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="47" t="s">
+        <v>148</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1250,14 +1372,16 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="47" t="s">
+        <v>151</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1280,34 +1404,48 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="47" t="s">
+        <v>150</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2">
         <v>6</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G9" s="46">
+        <v>45932</v>
+      </c>
+      <c r="H9" s="2">
+        <v>6</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="47" t="s">
+        <v>149</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1320,14 +1458,16 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="47" t="s">
+        <v>123</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1335,14 +1475,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="47" t="s">
+        <v>124</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1350,14 +1492,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="47" t="s">
+        <v>142</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1365,14 +1509,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="47" t="s">
+        <v>125</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1380,14 +1526,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="47" t="s">
+        <v>127</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1395,14 +1543,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="47" t="s">
+        <v>128</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1410,14 +1560,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="47" t="s">
+        <v>129</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1425,14 +1577,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="47" t="s">
+        <v>130</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1440,14 +1594,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="47" t="s">
+        <v>156</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1455,14 +1611,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="47" t="s">
+        <v>140</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1470,14 +1628,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="47" t="s">
+        <v>155</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>105</v>
       </c>
@@ -1485,14 +1645,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="47" t="s">
+        <v>132</v>
+      </c>
       <c r="D22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1500,14 +1662,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="47" t="s">
+        <v>157</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1515,14 +1679,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="47" t="s">
+        <v>131</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>14</v>
       </c>
@@ -1530,14 +1696,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="47" t="s">
+        <v>133</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>14</v>
       </c>
@@ -1545,14 +1713,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="47" t="s">
+        <v>135</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>48</v>
       </c>
@@ -1560,14 +1730,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="47" t="s">
+        <v>134</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>14</v>
       </c>
@@ -1575,14 +1747,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="47" t="s">
         <v>116</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -1599,7 +1771,7 @@
       <c r="B29" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="47" t="s">
         <v>117</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -1616,7 +1788,7 @@
       <c r="B30" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="47" t="s">
         <v>114</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -1626,14 +1798,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="47" t="s">
+        <v>152</v>
+      </c>
       <c r="D31" s="2" t="s">
         <v>22</v>
       </c>
@@ -1641,14 +1815,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="47" t="s">
+        <v>137</v>
+      </c>
       <c r="D32" s="2" t="s">
         <v>48</v>
       </c>
@@ -1656,14 +1832,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="47" t="s">
+        <v>136</v>
+      </c>
       <c r="D33" s="2" t="s">
         <v>44</v>
       </c>
@@ -1671,14 +1849,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="2"/>
+      <c r="C34" s="47" t="s">
+        <v>126</v>
+      </c>
       <c r="D34" s="2" t="s">
         <v>24</v>
       </c>
@@ -1686,14 +1866,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35" s="47" t="s">
+        <v>139</v>
+      </c>
       <c r="D35" s="2" t="s">
         <v>60</v>
       </c>
@@ -1701,14 +1883,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="2"/>
+      <c r="C36" s="47" t="s">
+        <v>138</v>
+      </c>
       <c r="D36" s="2" t="s">
         <v>48</v>
       </c>
@@ -1716,14 +1900,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="2"/>
+        <v>143</v>
+      </c>
+      <c r="C37" s="47" t="s">
+        <v>136</v>
+      </c>
       <c r="D37" s="2" t="s">
         <v>14</v>
       </c>
@@ -1731,14 +1917,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="3"/>
+      <c r="C38" s="47" t="s">
+        <v>153</v>
+      </c>
       <c r="D38" s="2" t="s">
         <v>24</v>
       </c>
@@ -1746,14 +1934,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="47" t="s">
+        <v>154</v>
+      </c>
       <c r="D39" s="2" t="s">
         <v>24</v>
       </c>
@@ -1776,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49D8E50-E16B-43C7-A737-D72E991DFD2E}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="117" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1794,39 +1984,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="7" t="s">
         <v>64</v>
       </c>
@@ -1844,7 +2034,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="29">
+      <c r="A4" s="26">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="str">
@@ -1855,25 +2045,25 @@
         <f>'Product backlog'!B3</f>
         <v>Instalar las herramientas de desarrollo</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="26">
         <v>6</v>
       </c>
       <c r="G4" s="2">
         <f>'Product backlog'!E3</f>
         <v>1</v>
       </c>
-      <c r="H4" s="29">
+      <c r="H4" s="26">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="2" t="str">
         <f>'Product backlog'!A4</f>
         <v>HT2</v>
@@ -1882,17 +2072,17 @@
         <f>'Product backlog'!B4</f>
         <v>Establecer el estándar de codificación</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="2">
         <f>'Product backlog'!E4</f>
         <v>1</v>
       </c>
-      <c r="H5" s="29"/>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="29"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="2" t="str">
         <f>'Product backlog'!A5</f>
         <v>HT3</v>
@@ -1901,14 +2091,14 @@
         <f>'Product backlog'!B5</f>
         <v>Establecer el diseño de base de datos</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="2">
         <f>'Product backlog'!E5</f>
         <v>6</v>
       </c>
-      <c r="H6" s="29"/>
+      <c r="H6" s="26"/>
       <c r="K6" s="2" t="s">
         <v>80</v>
       </c>
@@ -1918,7 +2108,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="29"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="2" t="str">
         <f>'Product backlog'!A6</f>
         <v>HT4</v>
@@ -1927,14 +2117,14 @@
         <f>'Product backlog'!B6</f>
         <v>Configurar los servidores y motores de lenguaje</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="2">
         <f>'Product backlog'!E6</f>
         <v>2</v>
       </c>
-      <c r="H7" s="29"/>
+      <c r="H7" s="26"/>
       <c r="K7" s="2" t="s">
         <v>70</v>
       </c>
@@ -1943,7 +2133,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="29"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="2" t="str">
         <f>'Product backlog'!A7</f>
         <v>HT5</v>
@@ -1952,14 +2142,14 @@
         <f>'Product backlog'!B7</f>
         <v>Configurar repositorio GitHub</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
       <c r="G8" s="2">
         <f>'Product backlog'!E7</f>
         <v>1</v>
       </c>
-      <c r="H8" s="29"/>
+      <c r="H8" s="26"/>
       <c r="K8" s="2" t="s">
         <v>71</v>
       </c>
@@ -1969,7 +2159,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="29"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="2" t="str">
         <f>'Product backlog'!A8</f>
         <v>HT6</v>
@@ -1978,17 +2168,17 @@
         <f>'Product backlog'!B8</f>
         <v>Implementar la base de datos</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
       <c r="G9" s="2">
         <f>'Product backlog'!E8</f>
         <v>1</v>
       </c>
-      <c r="H9" s="29"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="26">
+      <c r="A10" s="21">
         <v>2</v>
       </c>
       <c r="B10" s="10" t="str">
@@ -1999,25 +2189,25 @@
         <f>'Product backlog'!B9</f>
         <v>Establecer el diseño de las interfaces</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="27">
         <v>45363</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="19">
         <v>6</v>
       </c>
       <c r="G10" s="2">
         <f>'Product backlog'!E9</f>
         <v>6</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="19">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="10" t="str">
         <f>'Product backlog'!A10</f>
         <v>HT8</v>
@@ -2026,17 +2216,17 @@
         <f>'Product backlog'!B10</f>
         <v>Aprendizaje del framework FastAPI y React</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="39"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="2">
         <f>'Product backlog'!E10</f>
         <v>6</v>
       </c>
-      <c r="H11" s="39"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="26">
+      <c r="A12" s="21">
         <v>3</v>
       </c>
       <c r="B12" s="3" t="str">
@@ -2047,25 +2237,25 @@
         <f>'Product backlog'!B11</f>
         <v>Visualizar la página principal</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="17">
         <v>45363</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="17">
         <v>45577</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="21">
         <v>6</v>
       </c>
       <c r="G12" s="2">
         <f>'Product backlog'!E11</f>
         <v>3</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="21">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="3" t="str">
         <f>'Product backlog'!A12</f>
         <v>HU2</v>
@@ -2074,17 +2264,17 @@
         <f>'Product backlog'!B12</f>
         <v>Gestionar registro y autenticacion de usuarios</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="28"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="2">
         <f>'Product backlog'!E12</f>
         <v>9</v>
       </c>
-      <c r="H13" s="28"/>
+      <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="26">
+      <c r="A14" s="21">
         <v>4</v>
       </c>
       <c r="B14" s="3" t="str">
@@ -2095,25 +2285,25 @@
         <f>'Product backlog'!B13</f>
         <v>Reestablecer y actualizar contraseña</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="17">
         <v>45577</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="21">
         <v>6</v>
       </c>
       <c r="G14" s="2">
         <f>'Product backlog'!E13</f>
         <v>4</v>
       </c>
-      <c r="H14" s="26">
+      <c r="H14" s="21">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="27"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="3" t="str">
         <f>'Product backlog'!A14</f>
         <v>HU3</v>
@@ -2122,17 +2312,17 @@
         <f>'Product backlog'!B14</f>
         <v>Visualizar panel de inicio</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="27"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="32"/>
       <c r="G15" s="2">
         <f>'Product backlog'!E14</f>
         <v>2</v>
       </c>
-      <c r="H15" s="27"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="3" t="str">
         <f>'Product backlog'!A15</f>
         <v>HU5</v>
@@ -2141,17 +2331,17 @@
         <f>'Product backlog'!B15</f>
         <v>Gestionar membresías</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="28"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="22"/>
       <c r="G16" s="2">
         <f>'Product backlog'!E15</f>
         <v>8</v>
       </c>
-      <c r="H16" s="28"/>
+      <c r="H16" s="22"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="29">
+      <c r="A17" s="26">
         <v>5</v>
       </c>
       <c r="B17" s="3" t="str">
@@ -2162,25 +2352,25 @@
         <f>'Product backlog'!B16</f>
         <v>Visualizar membresías disponibles</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="26">
         <v>6</v>
       </c>
       <c r="G17" s="3">
         <f>'Product backlog'!E16</f>
         <v>2</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H17" s="26">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="29"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="3" t="str">
         <f>'Product backlog'!A17</f>
         <v>HU7</v>
@@ -2189,17 +2379,17 @@
         <f>'Product backlog'!B17</f>
         <v>Comprar membresía</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="29"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="26"/>
       <c r="G18" s="3">
         <f>'Product backlog'!E17</f>
         <v>6</v>
       </c>
-      <c r="H18" s="29"/>
+      <c r="H18" s="26"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="29"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="3" t="str">
         <f>'Product backlog'!A18</f>
         <v>HU8</v>
@@ -2208,17 +2398,17 @@
         <f>'Product backlog'!B18</f>
         <v>Visualizar estado de la membresía adquirida</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="29"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="26"/>
       <c r="G19" s="3">
         <f>'Product backlog'!E18</f>
         <v>2</v>
       </c>
-      <c r="H19" s="29"/>
+      <c r="H19" s="26"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="26">
+      <c r="A20" s="21">
         <v>6</v>
       </c>
       <c r="B20" s="3" t="str">
@@ -2229,25 +2419,25 @@
         <f>'Product backlog'!B19</f>
         <v>Implementación de JWT</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="21">
         <v>6</v>
       </c>
       <c r="G20" s="3">
         <f>'Product backlog'!E19</f>
         <v>6</v>
       </c>
-      <c r="H20" s="26">
+      <c r="H20" s="21">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="28"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="3" t="str">
         <f>'Product backlog'!A20</f>
         <v>HU20</v>
@@ -2256,17 +2446,17 @@
         <f>'Product backlog'!B20</f>
         <v>Gestionar categorías de gastos</v>
       </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="28"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="3">
         <f>'Product backlog'!E20</f>
         <v>5</v>
       </c>
-      <c r="H21" s="28"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="29">
+      <c r="A22" s="26">
         <v>7</v>
       </c>
       <c r="B22" s="3" t="str">
@@ -2277,25 +2467,25 @@
         <f>'Product backlog'!B21</f>
         <v>Redefinición de las tecnologías del front-end</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="33">
         <v>45839</v>
       </c>
-      <c r="F22" s="29">
+      <c r="F22" s="26">
         <v>6</v>
       </c>
       <c r="G22" s="3">
         <f>'Product backlog'!E21</f>
         <v>8</v>
       </c>
-      <c r="H22" s="29">
+      <c r="H22" s="26">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="29"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="4" t="str">
         <f>'Product backlog'!A22</f>
         <v>HU9</v>
@@ -2304,17 +2494,17 @@
         <f>'Product backlog'!B22</f>
         <v>Extraer comprobantes electrónicos</v>
       </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="29"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="26"/>
       <c r="G23" s="3">
         <f>'Product backlog'!E22</f>
         <v>10</v>
       </c>
-      <c r="H23" s="29"/>
+      <c r="H23" s="26"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="26">
+      <c r="A24" s="21">
         <v>8</v>
       </c>
       <c r="B24" s="3" t="str">
@@ -2325,25 +2515,25 @@
         <f>'Product backlog'!B23</f>
         <v>Diseñar diagrama de actividades</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="17">
         <v>45839</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="21">
         <v>6</v>
       </c>
       <c r="G24" s="2">
         <f>'Product backlog'!E23</f>
         <v>4</v>
       </c>
-      <c r="H24" s="26">
+      <c r="H24" s="21">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="27"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="3" t="str">
         <f>'Product backlog'!A24</f>
         <v>HU10</v>
@@ -2352,17 +2542,17 @@
         <f>'Product backlog'!B24</f>
         <v>Carga de comprobantes electrónicos</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="27"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="32"/>
       <c r="G25" s="2">
         <f>'Product backlog'!E24</f>
         <v>4</v>
       </c>
-      <c r="H25" s="27"/>
+      <c r="H25" s="32"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="27"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="3" t="str">
         <f>'Product backlog'!A25</f>
         <v>HU11</v>
@@ -2371,17 +2561,17 @@
         <f>'Product backlog'!B25</f>
         <v>Listar comprobantes cargados</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="27"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="32"/>
       <c r="G26" s="2">
         <f>'Product backlog'!E25</f>
         <v>4</v>
       </c>
-      <c r="H26" s="27"/>
+      <c r="H26" s="32"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="27"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="3" t="str">
         <f>'Product backlog'!A26</f>
         <v>HU13</v>
@@ -2390,17 +2580,17 @@
         <f>'Product backlog'!B26</f>
         <v>Visualizar detalles comprobante específico</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="27"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="2">
         <f>'Product backlog'!E26</f>
         <v>2</v>
       </c>
-      <c r="H27" s="27"/>
+      <c r="H27" s="32"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="28"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="3" t="str">
         <f>'Product backlog'!A27</f>
         <v>HU12</v>
@@ -2409,17 +2599,17 @@
         <f>'Product backlog'!B27</f>
         <v>Asignar categoría a los detalles del comprobante</v>
       </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="28"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="22"/>
       <c r="G28" s="2">
         <f>'Product backlog'!E27</f>
         <v>2</v>
       </c>
-      <c r="H28" s="28"/>
+      <c r="H28" s="22"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="26">
+      <c r="A29" s="21">
         <v>9</v>
       </c>
       <c r="B29" s="3" t="str">
@@ -2430,25 +2620,25 @@
         <f>'Product backlog'!B29</f>
         <v>Gestionar fracción básica desgravada</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="26">
+      <c r="F29" s="21">
         <v>6</v>
       </c>
       <c r="G29" s="2">
         <f>'Product backlog'!E29</f>
         <v>3</v>
       </c>
-      <c r="H29" s="26">
+      <c r="H29" s="21">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="27"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="3" t="str">
         <f>'Product backlog'!A30</f>
         <v>HU14</v>
@@ -2457,17 +2647,17 @@
         <f>'Product backlog'!B30</f>
         <v>Generar y Descargar Anexo de Gastos Personales</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
       <c r="G30" s="2">
         <f>'Product backlog'!E30</f>
         <v>8</v>
       </c>
-      <c r="H30" s="27"/>
+      <c r="H30" s="32"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="28"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="3" t="str">
         <f>'Product backlog'!A28</f>
         <v>HU21</v>
@@ -2476,17 +2666,17 @@
         <f>'Product backlog'!B28</f>
         <v>Gestionar Periodos Fiscales</v>
       </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
       <c r="G31" s="2">
         <f>'Product backlog'!E28</f>
         <v>4</v>
       </c>
-      <c r="H31" s="28"/>
+      <c r="H31" s="22"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="26">
+      <c r="A32" s="21">
         <v>10</v>
       </c>
       <c r="B32" s="3" t="str">
@@ -2497,25 +2687,25 @@
         <f>'Product backlog'!B31</f>
         <v>Implementar el modelo de machine learning</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="26">
+      <c r="F32" s="21">
         <v>5</v>
       </c>
       <c r="G32" s="2">
         <f>'Product backlog'!E31</f>
         <v>7</v>
       </c>
-      <c r="H32" s="26">
+      <c r="H32" s="21">
         <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="27"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="3" t="str">
         <f>'Product backlog'!A32</f>
         <v>HU16</v>
@@ -2524,17 +2714,17 @@
         <f>'Product backlog'!B32</f>
         <v>Visualizar predicción de gastos</v>
       </c>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="2">
         <f>'Product backlog'!E32</f>
         <v>7</v>
       </c>
-      <c r="H33" s="27"/>
+      <c r="H33" s="32"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="28"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="3" t="str">
         <f>'Product backlog'!A33</f>
         <v>HU15</v>
@@ -2543,165 +2733,186 @@
         <f>'Product backlog'!B33</f>
         <v>Configuración del Sistema - Intentos Login</v>
       </c>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
       <c r="G34" s="2">
         <f>'Product backlog'!E33</f>
         <v>4</v>
       </c>
-      <c r="H34" s="28"/>
+      <c r="H34" s="22"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="20">
+      <c r="A35" s="19">
         <v>11</v>
       </c>
-      <c r="B35" s="14" t="str">
+      <c r="B35" s="36" t="str">
         <f>'Product backlog'!A34</f>
         <v>HU4</v>
       </c>
-      <c r="C35" s="14" t="str">
+      <c r="C35" s="36" t="str">
         <f>'Product backlog'!B34</f>
         <v>Visualizar y modificar datos del usuario</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="D35" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="27">
         <v>45749</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F35" s="19">
         <v>6</v>
       </c>
-      <c r="G35" s="15">
+      <c r="G35" s="10">
         <f>'Product backlog'!E34</f>
         <v>3</v>
       </c>
-      <c r="H35" s="20">
+      <c r="H35" s="19">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="21"/>
-      <c r="B36" s="14" t="str">
+      <c r="A36" s="37"/>
+      <c r="B36" s="36" t="str">
         <f>'Product backlog'!A35</f>
         <v>HU18</v>
       </c>
-      <c r="C36" s="14" t="str">
+      <c r="C36" s="36" t="str">
         <f>'Product backlog'!B35</f>
         <v>Listar clientes registrados</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="15">
+      <c r="D36" s="37"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="10">
         <f>'Product backlog'!E35</f>
         <v>2</v>
       </c>
-      <c r="H36" s="21"/>
+      <c r="H36" s="37"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="21"/>
-      <c r="B37" s="14" t="str">
+      <c r="A37" s="37"/>
+      <c r="B37" s="36" t="str">
         <f>'Product backlog'!A36</f>
         <v>HU17</v>
       </c>
-      <c r="C37" s="14" t="str">
+      <c r="C37" s="36" t="str">
         <f>'Product backlog'!B36</f>
         <v>Visualizar y modificar datos del administrador</v>
       </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="15">
+      <c r="D37" s="37"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="10">
         <f>'Product backlog'!E36</f>
         <v>4</v>
       </c>
-      <c r="H37" s="21"/>
+      <c r="H37" s="37"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="22"/>
-      <c r="B38" s="14" t="str">
+      <c r="A38" s="20"/>
+      <c r="B38" s="36" t="str">
         <f>'Product backlog'!A37</f>
-        <v>HU22</v>
-      </c>
-      <c r="C38" s="14" t="str">
+        <v>HU23</v>
+      </c>
+      <c r="C38" s="36" t="str">
         <f>'Product backlog'!B37</f>
-        <v>Configuración y Modificación del Sistema - Tiempo sesion y Correo</v>
-      </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="15">
+        <v>Configuración del sistema - Tiempo sesion y Credenciales Correo</v>
+      </c>
+      <c r="D38" s="20"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="10">
         <f>'Product backlog'!E37</f>
         <v>6</v>
       </c>
-      <c r="H38" s="22"/>
+      <c r="H38" s="20"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="26">
+      <c r="A39" s="39">
         <v>12</v>
       </c>
-      <c r="B39" s="4" t="str">
+      <c r="B39" s="40" t="str">
         <f>'Product backlog'!A38</f>
         <v>HT10</v>
       </c>
-      <c r="C39" s="3" t="str">
+      <c r="C39" s="41" t="str">
         <f>'Product backlog'!B38</f>
         <v>Refactorización del código</v>
       </c>
-      <c r="D39" s="30">
+      <c r="D39" s="42">
         <v>45748</v>
       </c>
-      <c r="E39" s="30">
+      <c r="E39" s="42">
         <v>45901</v>
       </c>
-      <c r="F39" s="26">
+      <c r="F39" s="39">
         <v>5</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="43">
         <f>'Product backlog'!E38</f>
         <v>6</v>
       </c>
-      <c r="H39" s="26">
+      <c r="H39" s="39">
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="28"/>
-      <c r="B40" s="4" t="str">
+      <c r="A40" s="44"/>
+      <c r="B40" s="40" t="str">
         <f>'Product backlog'!A39</f>
         <v>HT11</v>
       </c>
-      <c r="C40" s="4" t="str">
+      <c r="C40" s="40" t="str">
         <f>'Product backlog'!B39</f>
         <v>Puesta a punto</v>
       </c>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="2">
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="43">
         <f>'Product backlog'!E39</f>
         <v>6</v>
       </c>
-      <c r="H40" s="28"/>
+      <c r="H40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="H4:H9"/>
-    <mergeCell ref="F4:F9"/>
-    <mergeCell ref="D4:D9"/>
-    <mergeCell ref="E4:E9"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="H35:H38"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="H24:H28"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="H39:H40"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A17:A19"/>
@@ -2718,41 +2929,20 @@
     <mergeCell ref="F14:F16"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H35:H38"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="H24:H28"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="H4:H9"/>
+    <mergeCell ref="F4:F9"/>
+    <mergeCell ref="D4:D9"/>
+    <mergeCell ref="E4:E9"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="F12:F13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>